<commit_message>
mod support design wip
</commit_message>
<xml_diff>
--- a/work_files/Pickaxe Power.xlsx
+++ b/work_files/Pickaxe Power.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="39">
   <si>
     <t>Pickaxe Power</t>
   </si>
@@ -92,9 +92,6 @@
     <t>Seconds take</t>
   </si>
   <si>
-    <t>Time to take one tile</t>
-  </si>
-  <si>
     <t>Swinging needed</t>
   </si>
   <si>
@@ -104,13 +101,7 @@
     <t>This is your input table</t>
   </si>
   <si>
-    <t>How many tiles can be taken before tool breaks</t>
-  </si>
-  <si>
     <t>Metal</t>
-  </si>
-  <si>
-    <t>Pick</t>
   </si>
   <si>
     <t>Time</t>
@@ -119,25 +110,53 @@
     <t>Count</t>
   </si>
   <si>
-    <t>Tool life</t>
-  </si>
-  <si>
     <t>Dirt</t>
   </si>
   <si>
     <t>Can be buffed</t>
+  </si>
+  <si>
+    <t>Red</t>
+  </si>
+  <si>
+    <t>Pickaxe</t>
+  </si>
+  <si>
+    <t>Tool life for tiles</t>
+  </si>
+  <si>
+    <t>Rows</t>
+  </si>
+  <si>
+    <t>Hatchet</t>
+  </si>
+  <si>
+    <t>AtkPoint</t>
+  </si>
+  <si>
+    <t>AtkPnt per second</t>
+  </si>
+  <si>
+    <t>AtkPnt per swing</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <i/>
@@ -208,8 +227,29 @@
       <name val="Raleway"/>
       <family val="3"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="2" tint="-0.749992370372631"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="2" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -232,8 +272,14 @@
         <fgColor rgb="FFF2F2F2"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -266,15 +312,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -289,49 +326,142 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="5"/>
-    <xf numFmtId="2" fontId="8" fillId="3" borderId="4" xfId="5" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="3" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="5"/>
+    <xf numFmtId="2" fontId="9" fillId="3" borderId="3" xfId="5" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="4" xfId="6"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="5"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="3" xfId="6"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="5"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="1" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="3" fillId="2" borderId="1" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="49" fontId="13" fillId="3" borderId="5" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="3" borderId="6" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="3" borderId="7" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="8" xfId="5" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="7" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="2" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="8">
+    <cellStyle name="20% - Accent3" xfId="7" builtinId="38"/>
     <cellStyle name="Calculation" xfId="6" builtinId="22"/>
     <cellStyle name="Explanatory Text" xfId="3" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="4" builtinId="19"/>
@@ -340,99 +470,52 @@
     <cellStyle name="Output" xfId="2" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="15">
     <dxf>
       <font>
         <b val="0"/>
-        <i val="0"/>
+        <i/>
         <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
-        <color rgb="FF000000"/>
+        <color theme="2" tint="-0.499984740745262"/>
         <name val="Calibri"/>
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor rgb="FFD9D9D9"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
         <b val="0"/>
-        <i val="0"/>
+        <i/>
         <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
-        <color theme="1"/>
+        <color theme="2" tint="-0.499984740745262"/>
         <name val="Calibri"/>
         <scheme val="none"/>
       </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor theme="0" tint="-0.14999847407452621"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
         <b val="0"/>
-        <i val="0"/>
+        <i/>
         <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
-        <color theme="1"/>
+        <color theme="2" tint="-0.499984740745262"/>
         <name val="Calibri"/>
         <scheme val="none"/>
       </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor theme="0" tint="-0.14999847407452621"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor theme="0" tint="-0.14999847407452621"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
@@ -449,25 +532,17 @@
     <dxf>
       <font>
         <b val="0"/>
-        <i val="0"/>
+        <i/>
         <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
-        <color rgb="FF000000"/>
+        <color theme="2" tint="-0.499984740745262"/>
         <name val="Calibri"/>
         <scheme val="none"/>
       </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor rgb="FFD9D9D9"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -492,27 +567,56 @@
       </fill>
     </dxf>
     <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
       <font>
-        <b val="0"/>
+        <b/>
         <i val="0"/>
         <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
-        <color theme="1"/>
+        <color theme="2" tint="-0.749992370372631"/>
         <name val="Calibri"/>
         <scheme val="none"/>
       </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="none">
-          <fgColor theme="0" tint="-0.14999847407452621"/>
-          <bgColor auto="1"/>
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
         </patternFill>
       </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1175,31 +1279,31 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>17.5</c:v>
+                  <c:v>12.25</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>41.25</c:v>
+                  <c:v>41.247895569215274</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>39.1875</c:v>
+                  <c:v>47.833333333333336</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>51.5625</c:v>
+                  <c:v>92.610482068116283</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>38.375</c:v>
+                  <c:v>79.75</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>71.395833333333329</c:v>
+                  <c:v>188.95369803208402</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>49.041666666666664</c:v>
+                  <c:v>181.77550256658165</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>87.895833333333329</c:v>
+                  <c:v>361.90744673189579</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>148.95833333333334</c:v>
+                  <c:v>840.50843987434189</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1396,7 +1500,7 @@
           <c:strCache>
             <c:ptCount val="1"/>
             <c:pt idx="0">
-              <c:v>Seconds take to break a oak plank</c:v>
+              <c:v>Seconds take to break a ebony plank</c:v>
             </c:pt>
           </c:strCache>
         </c:strRef>
@@ -1549,36 +1653,36 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sheet1 (2)'!$F$6:$F$14</c:f>
+              <c:f>Variables!$G$5:$G$13</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>1.3333333333333333</c:v>
+                  <c:v>1.5833333333333333</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.94280904158206325</c:v>
+                  <c:v>1.1195857368787001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.66666666666666663</c:v>
+                  <c:v>0.79166666666666663</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.59628479399994394</c:v>
+                  <c:v>0.70808819287493341</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.44444444444444442</c:v>
+                  <c:v>0.52777777777777779</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.35634832254989918</c:v>
+                  <c:v>0.42316363302800525</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.29095718698132317</c:v>
+                  <c:v>0.34551165954032126</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.23210354127426377</c:v>
+                  <c:v>0.27562295526318825</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.15823755442584711</c:v>
+                  <c:v>0.18790709588069343</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3414,13 +3518,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>190501</xdr:colOff>
+      <xdr:colOff>66675</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>128585</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>57151</xdr:colOff>
+      <xdr:colOff>114300</xdr:colOff>
       <xdr:row>38</xdr:row>
       <xdr:rowOff>180974</xdr:rowOff>
     </xdr:to>
@@ -3443,16 +3547,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>461961</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>80961</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>133349</xdr:rowOff>
+      <xdr:rowOff>123824</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>200024</xdr:colOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>180974</xdr:rowOff>
+      <xdr:rowOff>171449</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3516,7 +3620,7 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>128586</xdr:rowOff>
     </xdr:from>
@@ -3563,21 +3667,35 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A5:C14" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10" tableBorderDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A5:C14" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13" tableBorderDxfId="12">
   <autoFilter ref="A5:C14"/>
   <sortState ref="A6:B14">
     <sortCondition ref="B5:B14"/>
   </sortState>
   <tableColumns count="3">
-    <tableColumn id="1" name="Material" dataDxfId="8"/>
-    <tableColumn id="2" name="ForceMod" dataDxfId="7"/>
-    <tableColumn id="4" name="Durability" dataDxfId="1"/>
+    <tableColumn id="1" name="Material" dataDxfId="6" dataCellStyle="20% - Accent3"/>
+    <tableColumn id="2" name="ForceMod" dataCellStyle="Input"/>
+    <tableColumn id="4" name="Durability" dataDxfId="11"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleLight1" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="1" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table8" displayName="Table8" ref="L5:L14" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9" headerRowCellStyle="Explanatory Text" dataCellStyle="Output">
+  <autoFilter ref="L5:L14">
+    <filterColumn colId="0" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="1">
+    <tableColumn id="1" name="AtkPoint" dataDxfId="7" dataCellStyle="Output">
+      <calculatedColumnFormula>4*SQRT(Table3[[#This Row],[ForceMod]])*VLOOKUP($L$2,Variables!$A$3:$B$4,2,FALSE)</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table62" displayName="Table62" ref="E3:J4" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="6">
     <tableColumn id="1" name="Column1"/>
@@ -3591,29 +3709,29 @@
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table35" displayName="Table35" ref="A5:C14" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5" tableBorderDxfId="4">
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table35" displayName="Table35" ref="A5:C14" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4" tableBorderDxfId="3" dataCellStyle="Output">
   <autoFilter ref="A5:C14"/>
   <sortState ref="A6:B14">
     <sortCondition ref="B5:B14"/>
   </sortState>
   <tableColumns count="3">
-    <tableColumn id="1" name="Material" dataDxfId="3"/>
-    <tableColumn id="2" name="ForceMod" dataDxfId="2">
+    <tableColumn id="1" name="Material" dataDxfId="2" dataCellStyle="Output"/>
+    <tableColumn id="2" name="ForceMod" dataDxfId="1" dataCellStyle="Output">
       <calculatedColumnFormula>Table3[[#This Row],[ForceMod]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Durability" dataDxfId="0">
+    <tableColumn id="3" name="Durability" dataDxfId="0" dataCellStyle="Output">
       <calculatedColumnFormula>Table3[[#This Row],[Durability]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
-  <tableStyleInfo name="TableStyleLight1" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="1" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table7" displayName="Table7" ref="A1:B2" headerRowCount="0" totalsRowShown="0">
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table7" displayName="Table7" ref="A1:B4" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="2">
-    <tableColumn id="1" name="Name"/>
+    <tableColumn id="1" name="Name" dataDxfId="8"/>
     <tableColumn id="2" name="Value"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -3883,10 +4001,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q16"/>
+  <dimension ref="A1:S16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3894,84 +4012,89 @@
     <col min="1" max="2" width="12.85546875" customWidth="1"/>
     <col min="3" max="3" width="13.140625" customWidth="1"/>
     <col min="4" max="4" width="2.85546875" customWidth="1"/>
-    <col min="5" max="13" width="9.140625" customWidth="1"/>
+    <col min="5" max="10" width="9.140625" customWidth="1"/>
+    <col min="11" max="11" width="2.85546875" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" customWidth="1"/>
+    <col min="13" max="13" width="2.85546875" customWidth="1"/>
+    <col min="14" max="15" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="45" x14ac:dyDescent="0.6">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:19" ht="45" x14ac:dyDescent="0.6">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="E2" s="15" t="s">
+    <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E2" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="15"/>
-      <c r="G2" s="14">
-        <f>VLOOKUP(E2,Variables!1:1048576,2,FALSE)</f>
-        <v>3</v>
-      </c>
-      <c r="H2" s="7" t="s">
+      <c r="F2" s="12"/>
+      <c r="H2" s="4" t="s">
         <v>1</v>
       </c>
+      <c r="L2" s="23" t="s">
+        <v>37</v>
+      </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="8">
+      <c r="B3" s="5">
         <v>3</v>
       </c>
-      <c r="C3" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="E3" s="21" t="s">
+      <c r="C3" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="21" t="s">
+      <c r="F3" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="H3" s="21" t="s">
+      <c r="G3" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="H3" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="J3" s="21"/>
-      <c r="L3" s="21" t="str">
+      <c r="I3" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="J3" s="17"/>
+      <c r="K3" s="17"/>
+      <c r="L3" s="24"/>
+      <c r="N3" s="17" t="str">
         <f>Table6[[#This Row],[Column1]]</f>
         <v>Stone</v>
       </c>
-      <c r="M3" s="21" t="str">
+      <c r="O3" s="17" t="str">
         <f>Table6[[#This Row],[Column2]]</f>
         <v>Ice</v>
       </c>
-      <c r="N3" s="21" t="str">
+      <c r="P3" s="17" t="str">
         <f>Table6[[#This Row],[Column3]]</f>
         <v>Dirt</v>
       </c>
-      <c r="O3" s="21" t="str">
+      <c r="Q3" s="17" t="str">
         <f>Table6[[#This Row],[Column4]]</f>
         <v>Glass</v>
       </c>
-      <c r="P3" s="21" t="str">
+      <c r="R3" s="17" t="str">
         <f>Table6[[#This Row],[Column5]]</f>
         <v>Metal</v>
       </c>
-      <c r="Q3" s="21">
+      <c r="S3" s="17">
         <f>Table6[[#This Row],[Column6]]</f>
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
       <c r="E4">
         <v>48</v>
       </c>
@@ -3987,8 +4110,9 @@
       <c r="I4">
         <v>125</v>
       </c>
+      <c r="L4" s="25"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -3998,589 +4122,642 @@
       <c r="C5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="16"/>
-      <c r="J5" s="16"/>
-      <c r="L5" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="M5" s="19"/>
-      <c r="N5" s="19"/>
-      <c r="O5" s="19"/>
-      <c r="P5" s="19"/>
-      <c r="Q5" s="19"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="29" t="str">
+        <f>E2&amp;" to take one tile"</f>
+        <v>Seconds take to take one tile</v>
+      </c>
+      <c r="F5" s="29"/>
+      <c r="G5" s="29"/>
+      <c r="H5" s="29"/>
+      <c r="I5" s="29"/>
+      <c r="J5" s="29"/>
+      <c r="K5" s="18"/>
+      <c r="L5" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="N5" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="O5" s="30"/>
+      <c r="P5" s="30"/>
+      <c r="Q5" s="30"/>
+      <c r="R5" s="30"/>
+      <c r="S5" s="30"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="27">
         <v>1</v>
       </c>
-      <c r="C6">
-        <v>840</v>
-      </c>
-      <c r="E6" s="4">
-        <f>E$4/(4*$G$2*SQRT($B6))</f>
+      <c r="C6" s="11">
+        <f>ROUND(0.42*C7,0)</f>
+        <v>147</v>
+      </c>
+      <c r="E6" s="2">
+        <f>E$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B6))</f>
         <v>4</v>
       </c>
-      <c r="F6" s="4">
-        <f t="shared" ref="F6:J6" si="0">F$4/(4*$G$2*SQRT($B6))</f>
+      <c r="F6" s="2">
+        <f>F$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B6))</f>
         <v>2.9166666666666665</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="2">
+        <f>G$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B6))</f>
+        <v>2</v>
+      </c>
+      <c r="H6" s="2">
+        <f>H$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B6))</f>
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="I6" s="2">
+        <f>I$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B6))</f>
+        <v>10.416666666666666</v>
+      </c>
+      <c r="J6" s="2">
+        <f>J$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B6))</f>
+        <v>0</v>
+      </c>
+      <c r="L6" s="14">
+        <f>4*SQRT(Table3[[#This Row],[ForceMod]])*VLOOKUP($L$2,Variables!$A$3:$B$4,2,FALSE)</f>
+        <v>12</v>
+      </c>
+      <c r="N6" s="14">
+        <f>$C6/(E$4/(4*SQRT($B6)))</f>
+        <v>12.25</v>
+      </c>
+      <c r="O6" s="14">
+        <f t="shared" ref="O6:S6" si="0">$C6/(F$4/(4*SQRT($B6)))</f>
+        <v>16.8</v>
+      </c>
+      <c r="P6" s="14">
         <f t="shared" si="0"/>
+        <v>24.5</v>
+      </c>
+      <c r="Q6" s="14">
+        <f t="shared" si="0"/>
+        <v>117.6</v>
+      </c>
+      <c r="R6" s="14">
+        <f t="shared" si="0"/>
+        <v>4.7039999999999997</v>
+      </c>
+      <c r="S6" s="14" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="27">
         <v>2</v>
       </c>
-      <c r="H6" s="4">
-        <f t="shared" si="0"/>
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="I6" s="4">
-        <f t="shared" si="0"/>
-        <v>10.416666666666666</v>
-      </c>
-      <c r="J6" s="4">
-        <f t="shared" si="0"/>
+      <c r="C7" s="4">
+        <v>350</v>
+      </c>
+      <c r="E7" s="2">
+        <f>E$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B7))</f>
+        <v>2.8284271247461898</v>
+      </c>
+      <c r="F7" s="2">
+        <f>F$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B7))</f>
+        <v>2.0623947784607632</v>
+      </c>
+      <c r="G7" s="2">
+        <f>G$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B7))</f>
+        <v>1.4142135623730949</v>
+      </c>
+      <c r="H7" s="2">
+        <f>H$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B7))</f>
+        <v>0.29462782549439476</v>
+      </c>
+      <c r="I7" s="2">
+        <f>I$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B7))</f>
+        <v>7.3656956373598694</v>
+      </c>
+      <c r="J7" s="2">
+        <f>J$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B7))</f>
         <v>0</v>
       </c>
-      <c r="L6" s="18">
-        <f>$C6/E$4</f>
-        <v>17.5</v>
-      </c>
-      <c r="M6" s="18">
-        <f t="shared" ref="M6:Q14" si="1">$C6/F$4</f>
+      <c r="L7" s="14">
+        <f>4*SQRT(Table3[[#This Row],[ForceMod]])*VLOOKUP($L$2,Variables!$A$3:$B$4,2,FALSE)</f>
+        <v>16.970562748477143</v>
+      </c>
+      <c r="N7" s="14">
+        <f t="shared" ref="N7:N14" si="1">$C7/(E$4/(4*SQRT($B7)))</f>
+        <v>41.247895569215274</v>
+      </c>
+      <c r="O7" s="14">
+        <f t="shared" ref="O7:O14" si="2">$C7/(F$4/(4*SQRT($B7)))</f>
+        <v>56.568542494923811</v>
+      </c>
+      <c r="P7" s="14">
+        <f t="shared" ref="P7:P14" si="3">$C7/(G$4/(4*SQRT($B7)))</f>
+        <v>82.495791138430548</v>
+      </c>
+      <c r="Q7" s="14">
+        <f t="shared" ref="Q7:Q14" si="4">$C7/(H$4/(4*SQRT($B7)))</f>
+        <v>395.97979746446663</v>
+      </c>
+      <c r="R7" s="14">
+        <f t="shared" ref="R7:R14" si="5">$C7/(I$4/(4*SQRT($B7)))</f>
+        <v>15.839191898578667</v>
+      </c>
+      <c r="S7" s="14" t="e">
+        <f t="shared" ref="S7:S14" si="6">$C7/(J$4/(4*SQRT($B7)))</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="27">
+        <v>4</v>
+      </c>
+      <c r="C8" s="11">
+        <f>ROUND(0.82*C7,0)</f>
+        <v>287</v>
+      </c>
+      <c r="E8" s="2">
+        <f>E$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B8))</f>
+        <v>2</v>
+      </c>
+      <c r="F8" s="2">
+        <f>F$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B8))</f>
+        <v>1.4583333333333333</v>
+      </c>
+      <c r="G8" s="2">
+        <f>G$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B8))</f>
+        <v>1</v>
+      </c>
+      <c r="H8" s="2">
+        <f>H$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B8))</f>
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="I8" s="2">
+        <f>I$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B8))</f>
+        <v>5.208333333333333</v>
+      </c>
+      <c r="J8" s="2">
+        <f>J$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B8))</f>
+        <v>0</v>
+      </c>
+      <c r="L8" s="14">
+        <f>4*SQRT(Table3[[#This Row],[ForceMod]])*VLOOKUP($L$2,Variables!$A$3:$B$4,2,FALSE)</f>
         <v>24</v>
       </c>
-      <c r="N6" s="18">
+      <c r="N8" s="14">
         <f t="shared" si="1"/>
-        <v>35</v>
-      </c>
-      <c r="O6" s="18">
+        <v>47.833333333333336</v>
+      </c>
+      <c r="O8" s="14">
+        <f t="shared" si="2"/>
+        <v>65.599999999999994</v>
+      </c>
+      <c r="P8" s="14">
+        <f t="shared" si="3"/>
+        <v>95.666666666666671</v>
+      </c>
+      <c r="Q8" s="14">
+        <f t="shared" si="4"/>
+        <v>459.2</v>
+      </c>
+      <c r="R8" s="14">
+        <f t="shared" si="5"/>
+        <v>18.367999999999999</v>
+      </c>
+      <c r="S8" s="14" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="27">
+        <v>5</v>
+      </c>
+      <c r="C9" s="11">
+        <f>ROUND(1.42*C7,0)</f>
+        <v>497</v>
+      </c>
+      <c r="E9" s="2">
+        <f>E$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B9))</f>
+        <v>1.7888543819998317</v>
+      </c>
+      <c r="F9" s="2">
+        <f>F$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B9))</f>
+        <v>1.3043729868748772</v>
+      </c>
+      <c r="G9" s="2">
+        <f>G$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B9))</f>
+        <v>0.89442719099991586</v>
+      </c>
+      <c r="H9" s="2">
+        <f>H$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B9))</f>
+        <v>0.18633899812498247</v>
+      </c>
+      <c r="I9" s="2">
+        <f>I$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B9))</f>
+        <v>4.6584749531245615</v>
+      </c>
+      <c r="J9" s="2">
+        <f>J$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B9))</f>
+        <v>0</v>
+      </c>
+      <c r="L9" s="14">
+        <f>4*SQRT(Table3[[#This Row],[ForceMod]])*VLOOKUP($L$2,Variables!$A$3:$B$4,2,FALSE)</f>
+        <v>26.832815729997478</v>
+      </c>
+      <c r="N9" s="14">
         <f t="shared" si="1"/>
-        <v>168</v>
-      </c>
-      <c r="P6" s="18">
+        <v>92.610482068116283</v>
+      </c>
+      <c r="O9" s="14">
+        <f t="shared" si="2"/>
+        <v>127.00866112198807</v>
+      </c>
+      <c r="P9" s="14">
+        <f t="shared" si="3"/>
+        <v>185.22096413623257</v>
+      </c>
+      <c r="Q9" s="14">
+        <f t="shared" si="4"/>
+        <v>889.06062785391634</v>
+      </c>
+      <c r="R9" s="14">
+        <f t="shared" si="5"/>
+        <v>35.562425114156653</v>
+      </c>
+      <c r="S9" s="14" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="27">
+        <v>9</v>
+      </c>
+      <c r="C10" s="11">
+        <f>ROUND(0.91*C7,0)</f>
+        <v>319</v>
+      </c>
+      <c r="E10" s="2">
+        <f>E$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B10))</f>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="F10" s="2">
+        <f>F$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B10))</f>
+        <v>0.97222222222222221</v>
+      </c>
+      <c r="G10" s="2">
+        <f>G$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B10))</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="H10" s="2">
+        <f>H$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B10))</f>
+        <v>0.1388888888888889</v>
+      </c>
+      <c r="I10" s="2">
+        <f>I$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B10))</f>
+        <v>3.4722222222222223</v>
+      </c>
+      <c r="J10" s="2">
+        <f>J$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B10))</f>
+        <v>0</v>
+      </c>
+      <c r="L10" s="14">
+        <f>4*SQRT(Table3[[#This Row],[ForceMod]])*VLOOKUP($L$2,Variables!$A$3:$B$4,2,FALSE)</f>
+        <v>36</v>
+      </c>
+      <c r="N10" s="14">
         <f t="shared" si="1"/>
-        <v>6.72</v>
-      </c>
-      <c r="Q6" s="18" t="e">
+        <v>79.75</v>
+      </c>
+      <c r="O10" s="14">
+        <f t="shared" si="2"/>
+        <v>109.37142857142858</v>
+      </c>
+      <c r="P10" s="14">
+        <f t="shared" si="3"/>
+        <v>159.5</v>
+      </c>
+      <c r="Q10" s="14">
+        <f t="shared" si="4"/>
+        <v>765.6</v>
+      </c>
+      <c r="R10" s="14">
+        <f t="shared" si="5"/>
+        <v>30.624000000000002</v>
+      </c>
+      <c r="S10" s="14" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="27">
+        <v>14</v>
+      </c>
+      <c r="C11" s="11">
+        <f>ROUND(1.73*C7,0)</f>
+        <v>606</v>
+      </c>
+      <c r="E11" s="2">
+        <f>E$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B11))</f>
+        <v>1.0690449676496976</v>
+      </c>
+      <c r="F11" s="2">
+        <f>F$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B11))</f>
+        <v>0.77951195557790443</v>
+      </c>
+      <c r="G11" s="2">
+        <f>G$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B11))</f>
+        <v>0.53452248382484879</v>
+      </c>
+      <c r="H11" s="2">
+        <f>H$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B11))</f>
+        <v>0.11135885079684349</v>
+      </c>
+      <c r="I11" s="2">
+        <f>I$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B11))</f>
+        <v>2.7839712699210875</v>
+      </c>
+      <c r="J11" s="2">
+        <f>J$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B11))</f>
+        <v>0</v>
+      </c>
+      <c r="L11" s="14">
+        <f>4*SQRT(Table3[[#This Row],[ForceMod]])*VLOOKUP($L$2,Variables!$A$3:$B$4,2,FALSE)</f>
+        <v>44.899888641287298</v>
+      </c>
+      <c r="N11" s="14">
         <f t="shared" si="1"/>
+        <v>188.95369803208402</v>
+      </c>
+      <c r="O11" s="14">
+        <f t="shared" si="2"/>
+        <v>259.13650015828665</v>
+      </c>
+      <c r="P11" s="14">
+        <f t="shared" si="3"/>
+        <v>377.90739606416804</v>
+      </c>
+      <c r="Q11" s="14">
+        <f t="shared" si="4"/>
+        <v>1813.955501108007</v>
+      </c>
+      <c r="R11" s="14">
+        <f t="shared" si="5"/>
+        <v>72.558220044320265</v>
+      </c>
+      <c r="S11" s="14" t="e">
+        <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="3">
-        <v>2</v>
-      </c>
-      <c r="C7">
-        <v>1980</v>
-      </c>
-      <c r="E7" s="4">
-        <f t="shared" ref="E7:J14" si="2">E$4/(4*$G$2*SQRT($B7))</f>
-        <v>2.8284271247461898</v>
-      </c>
-      <c r="F7" s="4">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="27">
+        <v>21</v>
+      </c>
+      <c r="C12" s="11">
+        <f>ROUND(1.36*C7,0)</f>
+        <v>476</v>
+      </c>
+      <c r="E12" s="2">
+        <f>E$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B12))</f>
+        <v>0.87287156094396945</v>
+      </c>
+      <c r="F12" s="2">
+        <f>F$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B12))</f>
+        <v>0.63646884652164448</v>
+      </c>
+      <c r="G12" s="2">
+        <f>G$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B12))</f>
+        <v>0.43643578047198472</v>
+      </c>
+      <c r="H12" s="2">
+        <f>H$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B12))</f>
+        <v>9.0924120931663494E-2</v>
+      </c>
+      <c r="I12" s="2">
+        <f>I$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B12))</f>
+        <v>2.2731030232915872</v>
+      </c>
+      <c r="J12" s="2">
+        <f>J$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B12))</f>
+        <v>0</v>
+      </c>
+      <c r="L12" s="14">
+        <f>4*SQRT(Table3[[#This Row],[ForceMod]])*VLOOKUP($L$2,Variables!$A$3:$B$4,2,FALSE)</f>
+        <v>54.990908339470082</v>
+      </c>
+      <c r="N12" s="14">
+        <f t="shared" si="1"/>
+        <v>181.77550256658165</v>
+      </c>
+      <c r="O12" s="14">
         <f t="shared" si="2"/>
-        <v>2.0623947784607632</v>
-      </c>
-      <c r="G7" s="4">
+        <v>249.29211780559768</v>
+      </c>
+      <c r="P12" s="14">
+        <f t="shared" si="3"/>
+        <v>363.5510051331633</v>
+      </c>
+      <c r="Q12" s="14">
+        <f t="shared" si="4"/>
+        <v>1745.0448246391836</v>
+      </c>
+      <c r="R12" s="14">
+        <f t="shared" si="5"/>
+        <v>69.801792985567346</v>
+      </c>
+      <c r="S12" s="14" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="27">
+        <v>33</v>
+      </c>
+      <c r="C13" s="11">
+        <f>ROUND(2.16*C7,0)</f>
+        <v>756</v>
+      </c>
+      <c r="E13" s="2">
+        <f>E$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B13))</f>
+        <v>0.69631062382279141</v>
+      </c>
+      <c r="F13" s="2">
+        <f>F$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B13))</f>
+        <v>0.50772649653745205</v>
+      </c>
+      <c r="G13" s="2">
+        <f>G$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B13))</f>
+        <v>0.3481553119113957</v>
+      </c>
+      <c r="H13" s="2">
+        <f>H$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B13))</f>
+        <v>7.2532356648207438E-2</v>
+      </c>
+      <c r="I13" s="2">
+        <f>I$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B13))</f>
+        <v>1.8133089162051859</v>
+      </c>
+      <c r="J13" s="2">
+        <f>J$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B13))</f>
+        <v>0</v>
+      </c>
+      <c r="L13" s="14">
+        <f>4*SQRT(Table3[[#This Row],[ForceMod]])*VLOOKUP($L$2,Variables!$A$3:$B$4,2,FALSE)</f>
+        <v>68.934751758456343</v>
+      </c>
+      <c r="N13" s="14">
+        <f t="shared" si="1"/>
+        <v>361.90744673189579</v>
+      </c>
+      <c r="O13" s="14">
         <f t="shared" si="2"/>
-        <v>1.4142135623730949</v>
-      </c>
-      <c r="H7" s="4">
+        <v>496.33021266088571</v>
+      </c>
+      <c r="P13" s="14">
+        <f t="shared" si="3"/>
+        <v>723.81489346379158</v>
+      </c>
+      <c r="Q13" s="14">
+        <f t="shared" si="4"/>
+        <v>3474.3114886261997</v>
+      </c>
+      <c r="R13" s="14">
+        <f t="shared" si="5"/>
+        <v>138.97245954504797</v>
+      </c>
+      <c r="S13" s="14" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="27">
+        <v>71</v>
+      </c>
+      <c r="C14" s="11">
+        <f>ROUND(3.42*C7,0)</f>
+        <v>1197</v>
+      </c>
+      <c r="E14" s="2">
+        <f>E$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B14))</f>
+        <v>0.4747126632775413</v>
+      </c>
+      <c r="F14" s="2">
+        <f>F$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B14))</f>
+        <v>0.34614465030654051</v>
+      </c>
+      <c r="G14" s="2">
+        <f>G$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B14))</f>
+        <v>0.23735633163877065</v>
+      </c>
+      <c r="H14" s="2">
+        <f>H$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B14))</f>
+        <v>4.944923575807722E-2</v>
+      </c>
+      <c r="I14" s="2">
+        <f>I$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B14))</f>
+        <v>1.2362308939519304</v>
+      </c>
+      <c r="J14" s="2">
+        <f>J$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B14))</f>
+        <v>0</v>
+      </c>
+      <c r="L14" s="14">
+        <f>4*SQRT(Table3[[#This Row],[ForceMod]])*VLOOKUP($L$2,Variables!$A$3:$B$4,2,FALSE)</f>
+        <v>101.11379727811631</v>
+      </c>
+      <c r="N14" s="14">
+        <f t="shared" si="1"/>
+        <v>840.50843987434189</v>
+      </c>
+      <c r="O14" s="14">
         <f t="shared" si="2"/>
-        <v>0.29462782549439476</v>
-      </c>
-      <c r="I7" s="4">
-        <f t="shared" si="2"/>
-        <v>7.3656956373598694</v>
-      </c>
-      <c r="J7" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="L7" s="18">
-        <f t="shared" ref="L7:L14" si="3">$C7/E$4</f>
-        <v>41.25</v>
-      </c>
-      <c r="M7" s="18">
-        <f t="shared" si="1"/>
-        <v>56.571428571428569</v>
-      </c>
-      <c r="N7" s="18">
-        <f t="shared" si="1"/>
-        <v>82.5</v>
-      </c>
-      <c r="O7" s="18">
-        <f t="shared" si="1"/>
-        <v>396</v>
-      </c>
-      <c r="P7" s="18">
-        <f t="shared" si="1"/>
-        <v>15.84</v>
-      </c>
-      <c r="Q7" s="18" t="e">
-        <f t="shared" si="1"/>
+        <v>1152.697288970526</v>
+      </c>
+      <c r="P14" s="14">
+        <f t="shared" si="3"/>
+        <v>1681.0168797486838</v>
+      </c>
+      <c r="Q14" s="14">
+        <f t="shared" si="4"/>
+        <v>8068.881022793681</v>
+      </c>
+      <c r="R14" s="14">
+        <f t="shared" si="5"/>
+        <v>322.75524091174725</v>
+      </c>
+      <c r="S14" s="14" t="e">
+        <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="3">
-        <v>4</v>
-      </c>
-      <c r="C8">
-        <v>1881</v>
-      </c>
-      <c r="E8" s="4">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="F8" s="4">
-        <f t="shared" si="2"/>
-        <v>1.4583333333333333</v>
-      </c>
-      <c r="G8" s="4">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="H8" s="4">
-        <f t="shared" si="2"/>
-        <v>0.20833333333333334</v>
-      </c>
-      <c r="I8" s="4">
-        <f t="shared" si="2"/>
-        <v>5.208333333333333</v>
-      </c>
-      <c r="J8" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="L8" s="18">
-        <f t="shared" si="3"/>
-        <v>39.1875</v>
-      </c>
-      <c r="M8" s="18">
-        <f t="shared" si="1"/>
-        <v>53.74285714285714</v>
-      </c>
-      <c r="N8" s="18">
-        <f t="shared" si="1"/>
-        <v>78.375</v>
-      </c>
-      <c r="O8" s="18">
-        <f t="shared" si="1"/>
-        <v>376.2</v>
-      </c>
-      <c r="P8" s="18">
-        <f t="shared" si="1"/>
-        <v>15.048</v>
-      </c>
-      <c r="Q8" s="18" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A15" s="6"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="3">
-        <v>5</v>
-      </c>
-      <c r="C9">
-        <v>2475</v>
-      </c>
-      <c r="E9" s="4">
-        <f t="shared" si="2"/>
-        <v>1.7888543819998317</v>
-      </c>
-      <c r="F9" s="4">
-        <f t="shared" si="2"/>
-        <v>1.3043729868748772</v>
-      </c>
-      <c r="G9" s="4">
-        <f t="shared" si="2"/>
-        <v>0.89442719099991586</v>
-      </c>
-      <c r="H9" s="4">
-        <f t="shared" si="2"/>
-        <v>0.18633899812498247</v>
-      </c>
-      <c r="I9" s="4">
-        <f t="shared" si="2"/>
-        <v>4.6584749531245615</v>
-      </c>
-      <c r="J9" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="L9" s="18">
-        <f t="shared" si="3"/>
-        <v>51.5625</v>
-      </c>
-      <c r="M9" s="18">
-        <f t="shared" si="1"/>
-        <v>70.714285714285708</v>
-      </c>
-      <c r="N9" s="18">
-        <f t="shared" si="1"/>
-        <v>103.125</v>
-      </c>
-      <c r="O9" s="18">
-        <f t="shared" si="1"/>
-        <v>495</v>
-      </c>
-      <c r="P9" s="18">
-        <f t="shared" si="1"/>
-        <v>19.8</v>
-      </c>
-      <c r="Q9" s="18" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="3">
-        <v>9</v>
-      </c>
-      <c r="C10">
-        <v>1842</v>
-      </c>
-      <c r="E10" s="4">
-        <f t="shared" si="2"/>
-        <v>1.3333333333333333</v>
-      </c>
-      <c r="F10" s="4">
-        <f t="shared" si="2"/>
-        <v>0.97222222222222221</v>
-      </c>
-      <c r="G10" s="4">
-        <f t="shared" si="2"/>
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="H10" s="4">
-        <f t="shared" si="2"/>
-        <v>0.1388888888888889</v>
-      </c>
-      <c r="I10" s="4">
-        <f t="shared" si="2"/>
-        <v>3.4722222222222223</v>
-      </c>
-      <c r="J10" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="L10" s="18">
-        <f t="shared" si="3"/>
-        <v>38.375</v>
-      </c>
-      <c r="M10" s="18">
-        <f t="shared" si="1"/>
-        <v>52.628571428571426</v>
-      </c>
-      <c r="N10" s="18">
-        <f t="shared" si="1"/>
-        <v>76.75</v>
-      </c>
-      <c r="O10" s="18">
-        <f t="shared" si="1"/>
-        <v>368.4</v>
-      </c>
-      <c r="P10" s="18">
-        <f t="shared" si="1"/>
-        <v>14.736000000000001</v>
-      </c>
-      <c r="Q10" s="18" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="3">
-        <v>14</v>
-      </c>
-      <c r="C11">
-        <v>3427</v>
-      </c>
-      <c r="E11" s="4">
-        <f t="shared" si="2"/>
-        <v>1.0690449676496976</v>
-      </c>
-      <c r="F11" s="4">
-        <f t="shared" si="2"/>
-        <v>0.77951195557790443</v>
-      </c>
-      <c r="G11" s="4">
-        <f t="shared" si="2"/>
-        <v>0.53452248382484879</v>
-      </c>
-      <c r="H11" s="4">
-        <f t="shared" si="2"/>
-        <v>0.11135885079684349</v>
-      </c>
-      <c r="I11" s="4">
-        <f t="shared" si="2"/>
-        <v>2.7839712699210875</v>
-      </c>
-      <c r="J11" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="L11" s="18">
-        <f t="shared" si="3"/>
-        <v>71.395833333333329</v>
-      </c>
-      <c r="M11" s="18">
-        <f t="shared" si="1"/>
-        <v>97.914285714285711</v>
-      </c>
-      <c r="N11" s="18">
-        <f t="shared" si="1"/>
-        <v>142.79166666666666</v>
-      </c>
-      <c r="O11" s="18">
-        <f t="shared" si="1"/>
-        <v>685.4</v>
-      </c>
-      <c r="P11" s="18">
-        <f t="shared" si="1"/>
-        <v>27.416</v>
-      </c>
-      <c r="Q11" s="18" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="3">
+    <row r="16" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="str">
+        <f>"Attack points: 4 * sqrt(ForceMod) for each strike; "&amp;ROUND(B3,2)&amp;" strikes per second"</f>
+        <v>Attack points: 4 * sqrt(ForceMod) for each strike; 3 strikes per second</v>
+      </c>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="C12">
-        <v>2354</v>
-      </c>
-      <c r="E12" s="4">
-        <f t="shared" si="2"/>
-        <v>0.87287156094396945</v>
-      </c>
-      <c r="F12" s="4">
-        <f t="shared" si="2"/>
-        <v>0.63646884652164448</v>
-      </c>
-      <c r="G12" s="4">
-        <f t="shared" si="2"/>
-        <v>0.43643578047198472</v>
-      </c>
-      <c r="H12" s="4">
-        <f t="shared" si="2"/>
-        <v>9.0924120931663494E-2</v>
-      </c>
-      <c r="I12" s="4">
-        <f t="shared" si="2"/>
-        <v>2.2731030232915872</v>
-      </c>
-      <c r="J12" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="L12" s="18">
-        <f t="shared" si="3"/>
-        <v>49.041666666666664</v>
-      </c>
-      <c r="M12" s="18">
-        <f t="shared" si="1"/>
-        <v>67.257142857142853</v>
-      </c>
-      <c r="N12" s="18">
-        <f t="shared" si="1"/>
-        <v>98.083333333333329</v>
-      </c>
-      <c r="O12" s="18">
-        <f t="shared" si="1"/>
-        <v>470.8</v>
-      </c>
-      <c r="P12" s="18">
-        <f t="shared" si="1"/>
-        <v>18.832000000000001</v>
-      </c>
-      <c r="Q12" s="18" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13" s="3">
-        <v>33</v>
-      </c>
-      <c r="C13">
-        <v>4219</v>
-      </c>
-      <c r="E13" s="4">
-        <f t="shared" si="2"/>
-        <v>0.69631062382279141</v>
-      </c>
-      <c r="F13" s="4">
-        <f t="shared" si="2"/>
-        <v>0.50772649653745205</v>
-      </c>
-      <c r="G13" s="4">
-        <f t="shared" si="2"/>
-        <v>0.3481553119113957</v>
-      </c>
-      <c r="H13" s="4">
-        <f t="shared" si="2"/>
-        <v>7.2532356648207438E-2</v>
-      </c>
-      <c r="I13" s="4">
-        <f t="shared" si="2"/>
-        <v>1.8133089162051859</v>
-      </c>
-      <c r="J13" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="L13" s="18">
-        <f t="shared" si="3"/>
-        <v>87.895833333333329</v>
-      </c>
-      <c r="M13" s="18">
-        <f t="shared" si="1"/>
-        <v>120.54285714285714</v>
-      </c>
-      <c r="N13" s="18">
-        <f t="shared" si="1"/>
-        <v>175.79166666666666</v>
-      </c>
-      <c r="O13" s="18">
-        <f t="shared" si="1"/>
-        <v>843.8</v>
-      </c>
-      <c r="P13" s="18">
-        <f t="shared" si="1"/>
-        <v>33.752000000000002</v>
-      </c>
-      <c r="Q13" s="18" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="3">
-        <v>71</v>
-      </c>
-      <c r="C14">
-        <v>7150</v>
-      </c>
-      <c r="E14" s="4">
-        <f t="shared" si="2"/>
-        <v>0.4747126632775413</v>
-      </c>
-      <c r="F14" s="4">
-        <f t="shared" si="2"/>
-        <v>0.34614465030654051</v>
-      </c>
-      <c r="G14" s="4">
-        <f t="shared" si="2"/>
-        <v>0.23735633163877065</v>
-      </c>
-      <c r="H14" s="4">
-        <f t="shared" si="2"/>
-        <v>4.944923575807722E-2</v>
-      </c>
-      <c r="I14" s="4">
-        <f t="shared" si="2"/>
-        <v>1.2362308939519304</v>
-      </c>
-      <c r="J14" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="L14" s="18">
-        <f t="shared" si="3"/>
-        <v>148.95833333333334</v>
-      </c>
-      <c r="M14" s="18">
-        <f t="shared" si="1"/>
-        <v>204.28571428571428</v>
-      </c>
-      <c r="N14" s="18">
-        <f t="shared" si="1"/>
-        <v>297.91666666666669</v>
-      </c>
-      <c r="O14" s="18">
-        <f t="shared" si="1"/>
-        <v>1430</v>
-      </c>
-      <c r="P14" s="18">
-        <f t="shared" si="1"/>
-        <v>57.2</v>
-      </c>
-      <c r="Q14" s="18" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="9"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
-    </row>
-    <row r="16" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="11" t="str">
-        <f>"Attacks: 4 * sqrt(ForceMod) for each strike; "&amp;ROUND(B3,2)&amp;" strikes per second"</f>
-        <v>Attacks: 4 * sqrt(ForceMod) for each strike; 3 strikes per second</v>
-      </c>
-      <c r="B16" s="11"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="H16" s="11"/>
-      <c r="I16" s="11"/>
-      <c r="J16" s="11"/>
-      <c r="K16" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="L16" s="12"/>
-      <c r="M16" s="12"/>
-      <c r="N16" s="12"/>
+      <c r="M16" s="19"/>
+      <c r="N16" s="19"/>
+      <c r="O16" s="19"/>
+      <c r="P16" s="19"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="E5:J5"/>
-    <mergeCell ref="K16:N16"/>
     <mergeCell ref="A4:C4"/>
-    <mergeCell ref="L5:Q5"/>
+    <mergeCell ref="N5:S5"/>
+    <mergeCell ref="L16:P16"/>
+    <mergeCell ref="L2:L4"/>
     <mergeCell ref="A16:F16"/>
     <mergeCell ref="G16:J16"/>
   </mergeCells>
@@ -4592,18 +4769,25 @@
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75" bottom="0.75" header="0.30000000000000004" footer="0.30000000000000004"/>
   <pageSetup fitToWidth="0" fitToHeight="0" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
-  <tableParts count="2">
+  <tableParts count="3">
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Variables!$A$1:$A$2</xm:f>
           </x14:formula1>
           <xm:sqref>E2:F2</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Variables!$A$3:$A$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>L2</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -4616,7 +4800,7 @@
   <dimension ref="A1:Q16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M25" sqref="M25"/>
+      <selection activeCell="E2" sqref="E2:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4628,80 +4812,81 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="45" x14ac:dyDescent="0.6">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="3" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="15"/>
-      <c r="G2" s="14">
-        <f>VLOOKUP(E2,Variables!1:1048576,2,FALSE)</f>
-        <v>3</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>15</v>
+      <c r="F2" s="12"/>
+      <c r="H2" s="4" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="8">
+      <c r="B3" s="5">
         <v>3</v>
       </c>
-      <c r="E3" s="21" t="s">
+      <c r="E3" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="21" t="s">
+      <c r="F3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="21" t="s">
+      <c r="H3" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="21"/>
-      <c r="I3" s="21"/>
-      <c r="J3" s="21"/>
-      <c r="L3" s="21" t="str">
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
+      <c r="L3" s="17" t="str">
         <f>E3</f>
         <v>Ebony</v>
       </c>
-      <c r="M3" s="21" t="str">
+      <c r="M3" s="17" t="str">
         <f t="shared" ref="M3:Q3" si="0">F3</f>
+        <v>Red</v>
+      </c>
+      <c r="N3" s="17" t="str">
+        <f t="shared" si="0"/>
         <v>Oak</v>
       </c>
-      <c r="N3" s="21" t="str">
+      <c r="O3" s="17" t="str">
         <f t="shared" si="0"/>
         <v>Birch</v>
       </c>
-      <c r="O3" s="21">
+      <c r="P3" s="17">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="P3" s="21">
+      <c r="Q3" s="17">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q3" s="21">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
+      <c r="A4" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
       <c r="E4">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F4">
+        <v>17</v>
+      </c>
+      <c r="G4">
         <v>16</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>15</v>
       </c>
     </row>
@@ -4715,601 +4900,605 @@
       <c r="C5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="L5" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="M5" s="19"/>
-      <c r="N5" s="19"/>
-      <c r="O5" s="19"/>
-      <c r="P5" s="19"/>
-      <c r="Q5" s="19"/>
+      <c r="E5" s="29" t="str">
+        <f>E2&amp;" to take one tile"</f>
+        <v>Seconds take to take one tile</v>
+      </c>
+      <c r="F5" s="29"/>
+      <c r="G5" s="29"/>
+      <c r="H5" s="29"/>
+      <c r="I5" s="29"/>
+      <c r="J5" s="29"/>
+      <c r="L5" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="M5" s="30"/>
+      <c r="N5" s="30"/>
+      <c r="O5" s="30"/>
+      <c r="P5" s="30"/>
+      <c r="Q5" s="30"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="31">
         <f>Table3[[#This Row],[ForceMod]]</f>
         <v>1</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="31">
         <f>Table3[[#This Row],[Durability]]</f>
-        <v>840</v>
-      </c>
-      <c r="E6" s="4">
-        <f>E$4/(4*$G$2*SQRT($B6))</f>
-        <v>1.5</v>
-      </c>
-      <c r="F6" s="4">
-        <f t="shared" ref="F6:J6" si="1">F$4/(4*$G$2*SQRT($B6))</f>
+        <v>147</v>
+      </c>
+      <c r="E6" s="2">
+        <f>E$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B6))</f>
+        <v>1.5833333333333333</v>
+      </c>
+      <c r="F6" s="2">
+        <f>F$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B6))</f>
+        <v>1.4166666666666667</v>
+      </c>
+      <c r="G6" s="2">
+        <f>G$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B6))</f>
         <v>1.3333333333333333</v>
       </c>
-      <c r="G6" s="4">
+      <c r="H6" s="2">
+        <f>H$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B6))</f>
+        <v>1.25</v>
+      </c>
+      <c r="I6" s="2">
+        <f>I$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B6))</f>
+        <v>0</v>
+      </c>
+      <c r="J6" s="2">
+        <f>J$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B6))</f>
+        <v>0</v>
+      </c>
+      <c r="L6" s="14">
+        <f>$C6/E$4</f>
+        <v>7.7368421052631575</v>
+      </c>
+      <c r="M6" s="14">
+        <f t="shared" ref="M6:Q14" si="1">$C6/F$4</f>
+        <v>8.6470588235294112</v>
+      </c>
+      <c r="N6" s="14">
         <f t="shared" si="1"/>
-        <v>1.25</v>
-      </c>
-      <c r="H6" s="4">
+        <v>9.1875</v>
+      </c>
+      <c r="O6" s="14">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I6" s="4">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="P6" s="14" t="e">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J6" s="4">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q6" s="14" t="e">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L6" s="18">
-        <f>$C6/(E$4/(4*SQRT($B6)))</f>
-        <v>186.66666666666666</v>
-      </c>
-      <c r="M6" s="18">
-        <f t="shared" ref="M6:Q14" si="2">$C6/(F$4/(4*SQRT($B6)))</f>
-        <v>210</v>
-      </c>
-      <c r="N6" s="18">
-        <f t="shared" si="2"/>
-        <v>224</v>
-      </c>
-      <c r="O6" s="18" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P6" s="18" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q6" s="18" t="e">
-        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="31">
         <f>Table3[[#This Row],[ForceMod]]</f>
         <v>2</v>
       </c>
-      <c r="C7" s="10">
+      <c r="C7" s="31">
         <f>Table3[[#This Row],[Durability]]</f>
-        <v>1980</v>
-      </c>
-      <c r="E7" s="4">
-        <f t="shared" ref="E7:J14" si="3">E$4/(4*$G$2*SQRT($B7))</f>
-        <v>1.0606601717798212</v>
-      </c>
-      <c r="F7" s="4">
-        <f t="shared" si="3"/>
+        <v>350</v>
+      </c>
+      <c r="E7" s="2">
+        <f>E$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B7))</f>
+        <v>1.1195857368787001</v>
+      </c>
+      <c r="F7" s="2">
+        <f>F$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B7))</f>
+        <v>1.0017346066809423</v>
+      </c>
+      <c r="G7" s="2">
+        <f>G$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B7))</f>
         <v>0.94280904158206325</v>
       </c>
-      <c r="G7" s="4">
-        <f t="shared" si="3"/>
+      <c r="H7" s="2">
+        <f>H$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B7))</f>
         <v>0.88388347648318433</v>
       </c>
-      <c r="H7" s="4">
-        <f t="shared" si="3"/>
+      <c r="I7" s="2">
+        <f>I$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B7))</f>
         <v>0</v>
       </c>
-      <c r="I7" s="4">
-        <f t="shared" si="3"/>
+      <c r="J7" s="2">
+        <f>J$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B7))</f>
         <v>0</v>
       </c>
-      <c r="J7" s="4">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="L7" s="18">
-        <f t="shared" ref="L7:L14" si="4">$C7/(E$4/(4*SQRT($B7)))</f>
-        <v>622.25396744416184</v>
-      </c>
-      <c r="M7" s="18">
-        <f t="shared" si="2"/>
-        <v>700.03571337468213</v>
-      </c>
-      <c r="N7" s="18">
-        <f t="shared" si="2"/>
-        <v>746.7047609329943</v>
-      </c>
-      <c r="O7" s="18" t="e">
-        <f t="shared" si="2"/>
+      <c r="L7" s="14">
+        <f t="shared" ref="L7:L14" si="2">$C7/E$4</f>
+        <v>18.421052631578949</v>
+      </c>
+      <c r="M7" s="14">
+        <f t="shared" si="1"/>
+        <v>20.588235294117649</v>
+      </c>
+      <c r="N7" s="14">
+        <f t="shared" si="1"/>
+        <v>21.875</v>
+      </c>
+      <c r="O7" s="14">
+        <f t="shared" si="1"/>
+        <v>23.333333333333332</v>
+      </c>
+      <c r="P7" s="14" t="e">
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="P7" s="18" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q7" s="18" t="e">
-        <f t="shared" si="2"/>
+      <c r="Q7" s="14" t="e">
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="31">
         <f>Table3[[#This Row],[ForceMod]]</f>
         <v>4</v>
       </c>
-      <c r="C8" s="10">
+      <c r="C8" s="31">
         <f>Table3[[#This Row],[Durability]]</f>
-        <v>1881</v>
-      </c>
-      <c r="E8" s="4">
-        <f t="shared" si="3"/>
-        <v>0.75</v>
-      </c>
-      <c r="F8" s="4">
-        <f t="shared" si="3"/>
+        <v>287</v>
+      </c>
+      <c r="E8" s="2">
+        <f>E$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B8))</f>
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="F8" s="2">
+        <f>F$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B8))</f>
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="G8" s="2">
+        <f>G$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B8))</f>
         <v>0.66666666666666663</v>
       </c>
-      <c r="G8" s="4">
-        <f t="shared" si="3"/>
+      <c r="H8" s="2">
+        <f>H$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B8))</f>
         <v>0.625</v>
       </c>
-      <c r="H8" s="4">
-        <f t="shared" si="3"/>
+      <c r="I8" s="2">
+        <f>I$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B8))</f>
         <v>0</v>
       </c>
-      <c r="I8" s="4">
-        <f t="shared" si="3"/>
+      <c r="J8" s="2">
+        <f>J$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B8))</f>
         <v>0</v>
       </c>
-      <c r="J8" s="4">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="L8" s="18">
-        <f t="shared" si="4"/>
-        <v>836</v>
-      </c>
-      <c r="M8" s="18">
+      <c r="L8" s="14">
         <f t="shared" si="2"/>
-        <v>940.5</v>
-      </c>
-      <c r="N8" s="18">
-        <f t="shared" si="2"/>
-        <v>1003.2</v>
-      </c>
-      <c r="O8" s="18" t="e">
-        <f t="shared" si="2"/>
+        <v>15.105263157894736</v>
+      </c>
+      <c r="M8" s="14">
+        <f t="shared" si="1"/>
+        <v>16.882352941176471</v>
+      </c>
+      <c r="N8" s="14">
+        <f t="shared" si="1"/>
+        <v>17.9375</v>
+      </c>
+      <c r="O8" s="14">
+        <f t="shared" si="1"/>
+        <v>19.133333333333333</v>
+      </c>
+      <c r="P8" s="14" t="e">
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="P8" s="18" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q8" s="18" t="e">
-        <f t="shared" si="2"/>
+      <c r="Q8" s="14" t="e">
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="31">
         <f>Table3[[#This Row],[ForceMod]]</f>
         <v>5</v>
       </c>
-      <c r="C9" s="10">
+      <c r="C9" s="31">
         <f>Table3[[#This Row],[Durability]]</f>
-        <v>2475</v>
-      </c>
-      <c r="E9" s="4">
-        <f t="shared" si="3"/>
-        <v>0.67082039324993692</v>
-      </c>
-      <c r="F9" s="4">
-        <f t="shared" si="3"/>
+        <v>497</v>
+      </c>
+      <c r="E9" s="2">
+        <f>E$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B9))</f>
+        <v>0.70808819287493341</v>
+      </c>
+      <c r="F9" s="2">
+        <f>F$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B9))</f>
+        <v>0.63355259362494043</v>
+      </c>
+      <c r="G9" s="2">
+        <f>G$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B9))</f>
         <v>0.59628479399994394</v>
       </c>
-      <c r="G9" s="4">
-        <f t="shared" si="3"/>
+      <c r="H9" s="2">
+        <f>H$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B9))</f>
         <v>0.55901699437494745</v>
       </c>
-      <c r="H9" s="4">
-        <f t="shared" si="3"/>
+      <c r="I9" s="2">
+        <f>I$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B9))</f>
         <v>0</v>
       </c>
-      <c r="I9" s="4">
-        <f t="shared" si="3"/>
+      <c r="J9" s="2">
+        <f>J$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B9))</f>
         <v>0</v>
       </c>
-      <c r="J9" s="4">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="L9" s="18">
-        <f t="shared" si="4"/>
-        <v>1229.8373876248843</v>
-      </c>
-      <c r="M9" s="18">
+      <c r="L9" s="14">
         <f t="shared" si="2"/>
-        <v>1383.5670610779948</v>
-      </c>
-      <c r="N9" s="18">
-        <f t="shared" si="2"/>
-        <v>1475.8048651498614</v>
-      </c>
-      <c r="O9" s="18" t="e">
-        <f t="shared" si="2"/>
+        <v>26.157894736842106</v>
+      </c>
+      <c r="M9" s="14">
+        <f t="shared" si="1"/>
+        <v>29.235294117647058</v>
+      </c>
+      <c r="N9" s="14">
+        <f t="shared" si="1"/>
+        <v>31.0625</v>
+      </c>
+      <c r="O9" s="14">
+        <f t="shared" si="1"/>
+        <v>33.133333333333333</v>
+      </c>
+      <c r="P9" s="14" t="e">
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="P9" s="18" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q9" s="18" t="e">
-        <f t="shared" si="2"/>
+      <c r="Q9" s="14" t="e">
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="31">
         <f>Table3[[#This Row],[ForceMod]]</f>
         <v>9</v>
       </c>
-      <c r="C10" s="10">
+      <c r="C10" s="31">
         <f>Table3[[#This Row],[Durability]]</f>
-        <v>1842</v>
-      </c>
-      <c r="E10" s="4">
-        <f t="shared" si="3"/>
-        <v>0.5</v>
-      </c>
-      <c r="F10" s="4">
-        <f t="shared" si="3"/>
+        <v>319</v>
+      </c>
+      <c r="E10" s="2">
+        <f>E$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B10))</f>
+        <v>0.52777777777777779</v>
+      </c>
+      <c r="F10" s="2">
+        <f>F$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B10))</f>
+        <v>0.47222222222222221</v>
+      </c>
+      <c r="G10" s="2">
+        <f>G$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B10))</f>
         <v>0.44444444444444442</v>
       </c>
-      <c r="G10" s="4">
-        <f t="shared" si="3"/>
+      <c r="H10" s="2">
+        <f>H$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B10))</f>
         <v>0.41666666666666669</v>
       </c>
-      <c r="H10" s="4">
-        <f t="shared" si="3"/>
+      <c r="I10" s="2">
+        <f>I$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B10))</f>
         <v>0</v>
       </c>
-      <c r="I10" s="4">
-        <f t="shared" si="3"/>
+      <c r="J10" s="2">
+        <f>J$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B10))</f>
         <v>0</v>
       </c>
-      <c r="J10" s="4">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="L10" s="18">
-        <f t="shared" si="4"/>
-        <v>1228</v>
-      </c>
-      <c r="M10" s="18">
+      <c r="L10" s="14">
         <f t="shared" si="2"/>
-        <v>1381.5</v>
-      </c>
-      <c r="N10" s="18">
-        <f t="shared" si="2"/>
-        <v>1473.6</v>
-      </c>
-      <c r="O10" s="18" t="e">
-        <f t="shared" si="2"/>
+        <v>16.789473684210527</v>
+      </c>
+      <c r="M10" s="14">
+        <f t="shared" si="1"/>
+        <v>18.764705882352942</v>
+      </c>
+      <c r="N10" s="14">
+        <f t="shared" si="1"/>
+        <v>19.9375</v>
+      </c>
+      <c r="O10" s="14">
+        <f t="shared" si="1"/>
+        <v>21.266666666666666</v>
+      </c>
+      <c r="P10" s="14" t="e">
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="P10" s="18" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q10" s="18" t="e">
-        <f t="shared" si="2"/>
+      <c r="Q10" s="14" t="e">
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="31">
         <f>Table3[[#This Row],[ForceMod]]</f>
         <v>14</v>
       </c>
-      <c r="C11" s="10">
+      <c r="C11" s="31">
         <f>Table3[[#This Row],[Durability]]</f>
-        <v>3427</v>
-      </c>
-      <c r="E11" s="4">
-        <f t="shared" si="3"/>
-        <v>0.40089186286863659</v>
-      </c>
-      <c r="F11" s="4">
-        <f t="shared" si="3"/>
+        <v>606</v>
+      </c>
+      <c r="E11" s="2">
+        <f>E$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B11))</f>
+        <v>0.42316363302800525</v>
+      </c>
+      <c r="F11" s="2">
+        <f>F$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B11))</f>
+        <v>0.37862009270926789</v>
+      </c>
+      <c r="G11" s="2">
+        <f>G$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B11))</f>
         <v>0.35634832254989918</v>
       </c>
-      <c r="G11" s="4">
-        <f t="shared" si="3"/>
+      <c r="H11" s="2">
+        <f>H$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B11))</f>
         <v>0.33407655239053047</v>
       </c>
-      <c r="H11" s="4">
-        <f t="shared" si="3"/>
+      <c r="I11" s="2">
+        <f>I$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B11))</f>
         <v>0</v>
       </c>
-      <c r="I11" s="4">
-        <f t="shared" si="3"/>
+      <c r="J11" s="2">
+        <f>J$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B11))</f>
         <v>0</v>
       </c>
-      <c r="J11" s="4">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="L11" s="18">
-        <f t="shared" si="4"/>
-        <v>2849.4799698831771</v>
-      </c>
-      <c r="M11" s="18">
+      <c r="L11" s="14">
         <f t="shared" si="2"/>
-        <v>3205.6649661185743</v>
-      </c>
-      <c r="N11" s="18">
-        <f t="shared" si="2"/>
-        <v>3419.3759638598126</v>
-      </c>
-      <c r="O11" s="18" t="e">
-        <f t="shared" si="2"/>
+        <v>31.894736842105264</v>
+      </c>
+      <c r="M11" s="14">
+        <f t="shared" si="1"/>
+        <v>35.647058823529413</v>
+      </c>
+      <c r="N11" s="14">
+        <f t="shared" si="1"/>
+        <v>37.875</v>
+      </c>
+      <c r="O11" s="14">
+        <f t="shared" si="1"/>
+        <v>40.4</v>
+      </c>
+      <c r="P11" s="14" t="e">
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="P11" s="18" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q11" s="18" t="e">
-        <f t="shared" si="2"/>
+      <c r="Q11" s="14" t="e">
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="31">
         <f>Table3[[#This Row],[ForceMod]]</f>
         <v>21</v>
       </c>
-      <c r="C12" s="10">
+      <c r="C12" s="31">
         <f>Table3[[#This Row],[Durability]]</f>
-        <v>2354</v>
-      </c>
-      <c r="E12" s="4">
-        <f t="shared" si="3"/>
-        <v>0.32732683535398854</v>
-      </c>
-      <c r="F12" s="4">
-        <f t="shared" si="3"/>
+        <v>476</v>
+      </c>
+      <c r="E12" s="2">
+        <f>E$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B12))</f>
+        <v>0.34551165954032126</v>
+      </c>
+      <c r="F12" s="2">
+        <f>F$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B12))</f>
+        <v>0.30914201116765588</v>
+      </c>
+      <c r="G12" s="2">
+        <f>G$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B12))</f>
         <v>0.29095718698132317</v>
       </c>
-      <c r="G12" s="4">
-        <f t="shared" si="3"/>
+      <c r="H12" s="2">
+        <f>H$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B12))</f>
         <v>0.27277236279499045</v>
       </c>
-      <c r="H12" s="4">
-        <f t="shared" si="3"/>
+      <c r="I12" s="2">
+        <f>I$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B12))</f>
         <v>0</v>
       </c>
-      <c r="I12" s="4">
-        <f t="shared" si="3"/>
+      <c r="J12" s="2">
+        <f>J$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B12))</f>
         <v>0</v>
       </c>
-      <c r="J12" s="4">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="L12" s="18">
-        <f t="shared" si="4"/>
-        <v>2397.1962635391214</v>
-      </c>
-      <c r="M12" s="18">
+      <c r="L12" s="14">
         <f t="shared" si="2"/>
-        <v>2696.8457964815116</v>
-      </c>
-      <c r="N12" s="18">
-        <f t="shared" si="2"/>
-        <v>2876.6355162469458</v>
-      </c>
-      <c r="O12" s="18" t="e">
-        <f t="shared" si="2"/>
+        <v>25.05263157894737</v>
+      </c>
+      <c r="M12" s="14">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="N12" s="14">
+        <f t="shared" si="1"/>
+        <v>29.75</v>
+      </c>
+      <c r="O12" s="14">
+        <f t="shared" si="1"/>
+        <v>31.733333333333334</v>
+      </c>
+      <c r="P12" s="14" t="e">
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="P12" s="18" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q12" s="18" t="e">
-        <f t="shared" si="2"/>
+      <c r="Q12" s="14" t="e">
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13" s="31">
         <f>Table3[[#This Row],[ForceMod]]</f>
         <v>33</v>
       </c>
-      <c r="C13" s="10">
+      <c r="C13" s="31">
         <f>Table3[[#This Row],[Durability]]</f>
-        <v>4219</v>
-      </c>
-      <c r="E13" s="4">
-        <f t="shared" si="3"/>
-        <v>0.26111648393354675</v>
-      </c>
-      <c r="F13" s="4">
-        <f t="shared" si="3"/>
+        <v>756</v>
+      </c>
+      <c r="E13" s="2">
+        <f>E$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B13))</f>
+        <v>0.27562295526318825</v>
+      </c>
+      <c r="F13" s="2">
+        <f>F$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B13))</f>
+        <v>0.24661001260390528</v>
+      </c>
+      <c r="G13" s="2">
+        <f>G$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B13))</f>
         <v>0.23210354127426377</v>
       </c>
-      <c r="G13" s="4">
-        <f t="shared" si="3"/>
+      <c r="H13" s="2">
+        <f>H$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B13))</f>
         <v>0.2175970699446223</v>
       </c>
-      <c r="H13" s="4">
-        <f t="shared" si="3"/>
+      <c r="I13" s="2">
+        <f>I$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B13))</f>
         <v>0</v>
       </c>
-      <c r="I13" s="4">
-        <f t="shared" si="3"/>
+      <c r="J13" s="2">
+        <f>J$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B13))</f>
         <v>0</v>
       </c>
-      <c r="J13" s="4">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="L13" s="18">
-        <f t="shared" si="4"/>
-        <v>5385.8466234986536</v>
-      </c>
-      <c r="M13" s="18">
+      <c r="L13" s="14">
         <f t="shared" si="2"/>
-        <v>6059.0774514359855</v>
-      </c>
-      <c r="N13" s="18">
-        <f t="shared" si="2"/>
-        <v>6463.0159481983856</v>
-      </c>
-      <c r="O13" s="18" t="e">
-        <f t="shared" si="2"/>
+        <v>39.789473684210527</v>
+      </c>
+      <c r="M13" s="14">
+        <f t="shared" si="1"/>
+        <v>44.470588235294116</v>
+      </c>
+      <c r="N13" s="14">
+        <f t="shared" si="1"/>
+        <v>47.25</v>
+      </c>
+      <c r="O13" s="14">
+        <f t="shared" si="1"/>
+        <v>50.4</v>
+      </c>
+      <c r="P13" s="14" t="e">
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="P13" s="18" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q13" s="18" t="e">
-        <f t="shared" si="2"/>
+      <c r="Q13" s="14" t="e">
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="31">
         <f>Table3[[#This Row],[ForceMod]]</f>
         <v>71</v>
       </c>
-      <c r="C14" s="10">
+      <c r="C14" s="31">
         <f>Table3[[#This Row],[Durability]]</f>
-        <v>7150</v>
-      </c>
-      <c r="E14" s="4">
-        <f t="shared" si="3"/>
-        <v>0.17801724872907798</v>
-      </c>
-      <c r="F14" s="4">
-        <f t="shared" si="3"/>
+        <v>1197</v>
+      </c>
+      <c r="E14" s="2">
+        <f>E$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B14))</f>
+        <v>0.18790709588069343</v>
+      </c>
+      <c r="F14" s="2">
+        <f>F$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B14))</f>
+        <v>0.16812740157746256</v>
+      </c>
+      <c r="G14" s="2">
+        <f>G$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B14))</f>
         <v>0.15823755442584711</v>
       </c>
-      <c r="G14" s="4">
-        <f t="shared" si="3"/>
+      <c r="H14" s="2">
+        <f>H$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B14))</f>
         <v>0.14834770727423166</v>
       </c>
-      <c r="H14" s="4">
-        <f t="shared" si="3"/>
+      <c r="I14" s="2">
+        <f>I$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B14))</f>
         <v>0</v>
       </c>
-      <c r="I14" s="4">
-        <f t="shared" si="3"/>
+      <c r="J14" s="2">
+        <f>J$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B14))</f>
         <v>0</v>
       </c>
-      <c r="J14" s="4">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="L14" s="18">
-        <f t="shared" si="4"/>
-        <v>13388.215750713549</v>
-      </c>
-      <c r="M14" s="18">
+      <c r="L14" s="14">
         <f t="shared" si="2"/>
-        <v>15061.742719552742</v>
-      </c>
-      <c r="N14" s="18">
-        <f t="shared" si="2"/>
-        <v>16065.858900856259</v>
-      </c>
-      <c r="O14" s="18" t="e">
-        <f t="shared" si="2"/>
+        <v>63</v>
+      </c>
+      <c r="M14" s="14">
+        <f t="shared" si="1"/>
+        <v>70.411764705882348</v>
+      </c>
+      <c r="N14" s="14">
+        <f t="shared" si="1"/>
+        <v>74.8125</v>
+      </c>
+      <c r="O14" s="14">
+        <f t="shared" si="1"/>
+        <v>79.8</v>
+      </c>
+      <c r="P14" s="14" t="e">
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="P14" s="18" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q14" s="18" t="e">
-        <f t="shared" si="2"/>
+      <c r="Q14" s="14" t="e">
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="11" t="str">
+      <c r="A16" s="7" t="str">
         <f>"Attacks: 4 * sqrt(ForceMod) for each strike; "&amp;ROUND(B3,2)&amp;" strikes per second"</f>
         <v>Attacks: 4 * sqrt(ForceMod) for each strike; 3 strikes per second</v>
       </c>
-      <c r="B16" s="11"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11" t="s">
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="H16" s="11"/>
-      <c r="I16" s="11"/>
-      <c r="J16" s="11"/>
-      <c r="K16" s="11" t="s">
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="L16" s="11"/>
-      <c r="M16" s="11"/>
-      <c r="N16" s="11"/>
+      <c r="L16" s="7"/>
+      <c r="M16" s="7"/>
+      <c r="N16" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
     <mergeCell ref="A16:F16"/>
     <mergeCell ref="G16:J16"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="A4:C4"/>
     <mergeCell ref="K16:N16"/>
     <mergeCell ref="L5:Q5"/>
+    <mergeCell ref="E5:J5"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2">
@@ -5340,187 +5529,292 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.42578125" style="13" customWidth="1"/>
+    <col min="1" max="1" width="27.42578125" style="22" customWidth="1"/>
     <col min="2" max="2" width="9.140625" customWidth="1"/>
     <col min="4" max="5" width="9.140625" customWidth="1"/>
     <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="21" t="s">
         <v>22</v>
       </c>
       <c r="B1">
         <f>Sheet1!B3</f>
         <v>3</v>
       </c>
-      <c r="D1" s="14" t="str">
+      <c r="D1" s="11" t="str">
         <f>Sheet1!E2&amp;" to break a "&amp;LOWER(Sheet1!H2)&amp;" tile"</f>
         <v>Seconds take to break a stone tile</v>
       </c>
-      <c r="E1" s="14" t="str">
+      <c r="E1" s="11" t="str">
         <f>"Tool life for "&amp;LOWER(Sheet1!H2)&amp;" tiles"</f>
         <v>Tool life for stone tiles</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>24</v>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="21" t="s">
+        <v>23</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="D2" s="14" t="str">
+      <c r="D2" s="11" t="str">
         <f>'Sheet1 (2)'!E2&amp;" to break a "&amp;LOWER('Sheet1 (2)'!H2)&amp;" plank"</f>
-        <v>Seconds take to break a oak plank</v>
-      </c>
-      <c r="E2" s="14" t="str">
+        <v>Seconds take to break a ebony plank</v>
+      </c>
+      <c r="E2" s="11" t="str">
         <f>"Tool life for "&amp;LOWER('Sheet1 (2)'!H2)&amp;" tiles"</f>
-        <v>Tool life for oak tiles</v>
+        <v>Tool life for ebony tiles</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D4" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="E4" s="20" t="s">
-        <v>30</v>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="10">
+        <f>Sheet1!B3</f>
+        <v>3</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="H3" s="15"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>27</v>
       </c>
       <c r="F4" t="s">
-        <v>31</v>
+        <v>28</v>
+      </c>
+      <c r="G4" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" t="s">
+        <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D5" s="14">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D5" s="11">
         <v>4</v>
       </c>
-      <c r="E5" s="18">
+      <c r="E5" s="14">
         <f>HLOOKUP(Sheet1!$H$2,Sheet1!$E$3:$J$14,$D5,FALSE)</f>
         <v>4</v>
       </c>
-      <c r="F5" s="18">
-        <f>HLOOKUP(Sheet1!$H$2,Sheet1!$L$3:$Q$14,$D5,FALSE)</f>
-        <v>17.5</v>
+      <c r="F5" s="14">
+        <f>HLOOKUP(Sheet1!$H$2,Sheet1!$N$3:$S$14,$D5,FALSE)</f>
+        <v>12.25</v>
+      </c>
+      <c r="G5" s="14">
+        <f>HLOOKUP('Sheet1 (2)'!$H$2,'Sheet1 (2)'!$E$3:$J$14,$D5,FALSE)</f>
+        <v>1.5833333333333333</v>
+      </c>
+      <c r="H5" s="14" t="e">
+        <f>HLOOKUP('Sheet1 (2)'!$H$2,'Sheet1 (2)'!$N$3:$S$14,$D5,FALSE)</f>
+        <v>#N/A</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D6" s="14">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D6" s="11">
         <v>5</v>
       </c>
-      <c r="E6" s="18">
+      <c r="E6" s="14">
         <f>HLOOKUP(Sheet1!$H$2,Sheet1!$E$3:$J$14,$D6,FALSE)</f>
         <v>2.8284271247461898</v>
       </c>
-      <c r="F6" s="18">
-        <f>HLOOKUP(Sheet1!$H$2,Sheet1!$L$3:$Q$14,$D6,FALSE)</f>
-        <v>41.25</v>
+      <c r="F6" s="14">
+        <f>HLOOKUP(Sheet1!$H$2,Sheet1!$N$3:$S$14,$D6,FALSE)</f>
+        <v>41.247895569215274</v>
+      </c>
+      <c r="G6" s="14">
+        <f>HLOOKUP('Sheet1 (2)'!$H$2,'Sheet1 (2)'!$E$3:$J$14,$D6,FALSE)</f>
+        <v>1.1195857368787001</v>
+      </c>
+      <c r="H6" s="14" t="e">
+        <f>HLOOKUP('Sheet1 (2)'!$H$2,'Sheet1 (2)'!$N$3:$S$14,$D6,FALSE)</f>
+        <v>#N/A</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D7" s="14">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D7" s="11">
         <v>6</v>
       </c>
-      <c r="E7" s="18">
+      <c r="E7" s="14">
         <f>HLOOKUP(Sheet1!$H$2,Sheet1!$E$3:$J$14,$D7,FALSE)</f>
         <v>2</v>
       </c>
-      <c r="F7" s="18">
-        <f>HLOOKUP(Sheet1!$H$2,Sheet1!$L$3:$Q$14,$D7,FALSE)</f>
-        <v>39.1875</v>
+      <c r="F7" s="14">
+        <f>HLOOKUP(Sheet1!$H$2,Sheet1!$N$3:$S$14,$D7,FALSE)</f>
+        <v>47.833333333333336</v>
+      </c>
+      <c r="G7" s="14">
+        <f>HLOOKUP('Sheet1 (2)'!$H$2,'Sheet1 (2)'!$E$3:$J$14,$D7,FALSE)</f>
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="H7" s="14" t="e">
+        <f>HLOOKUP('Sheet1 (2)'!$H$2,'Sheet1 (2)'!$N$3:$S$14,$D7,FALSE)</f>
+        <v>#N/A</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D8" s="14">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D8" s="11">
         <v>7</v>
       </c>
-      <c r="E8" s="18">
+      <c r="E8" s="14">
         <f>HLOOKUP(Sheet1!$H$2,Sheet1!$E$3:$J$14,$D8,FALSE)</f>
         <v>1.7888543819998317</v>
       </c>
-      <c r="F8" s="18">
-        <f>HLOOKUP(Sheet1!$H$2,Sheet1!$L$3:$Q$14,$D8,FALSE)</f>
-        <v>51.5625</v>
+      <c r="F8" s="14">
+        <f>HLOOKUP(Sheet1!$H$2,Sheet1!$N$3:$S$14,$D8,FALSE)</f>
+        <v>92.610482068116283</v>
+      </c>
+      <c r="G8" s="14">
+        <f>HLOOKUP('Sheet1 (2)'!$H$2,'Sheet1 (2)'!$E$3:$J$14,$D8,FALSE)</f>
+        <v>0.70808819287493341</v>
+      </c>
+      <c r="H8" s="14" t="e">
+        <f>HLOOKUP('Sheet1 (2)'!$H$2,'Sheet1 (2)'!$N$3:$S$14,$D8,FALSE)</f>
+        <v>#N/A</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D9" s="14">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D9" s="11">
         <v>8</v>
       </c>
-      <c r="E9" s="18">
+      <c r="E9" s="14">
         <f>HLOOKUP(Sheet1!$H$2,Sheet1!$E$3:$J$14,$D9,FALSE)</f>
         <v>1.3333333333333333</v>
       </c>
-      <c r="F9" s="18">
-        <f>HLOOKUP(Sheet1!$H$2,Sheet1!$L$3:$Q$14,$D9,FALSE)</f>
-        <v>38.375</v>
+      <c r="F9" s="14">
+        <f>HLOOKUP(Sheet1!$H$2,Sheet1!$N$3:$S$14,$D9,FALSE)</f>
+        <v>79.75</v>
+      </c>
+      <c r="G9" s="14">
+        <f>HLOOKUP('Sheet1 (2)'!$H$2,'Sheet1 (2)'!$E$3:$J$14,$D9,FALSE)</f>
+        <v>0.52777777777777779</v>
+      </c>
+      <c r="H9" s="14" t="e">
+        <f>HLOOKUP('Sheet1 (2)'!$H$2,'Sheet1 (2)'!$N$3:$S$14,$D9,FALSE)</f>
+        <v>#N/A</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D10" s="14">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D10" s="11">
         <v>9</v>
       </c>
-      <c r="E10" s="18">
+      <c r="E10" s="14">
         <f>HLOOKUP(Sheet1!$H$2,Sheet1!$E$3:$J$14,$D10,FALSE)</f>
         <v>1.0690449676496976</v>
       </c>
-      <c r="F10" s="18">
-        <f>HLOOKUP(Sheet1!$H$2,Sheet1!$L$3:$Q$14,$D10,FALSE)</f>
-        <v>71.395833333333329</v>
+      <c r="F10" s="14">
+        <f>HLOOKUP(Sheet1!$H$2,Sheet1!$N$3:$S$14,$D10,FALSE)</f>
+        <v>188.95369803208402</v>
+      </c>
+      <c r="G10" s="14">
+        <f>HLOOKUP('Sheet1 (2)'!$H$2,'Sheet1 (2)'!$E$3:$J$14,$D10,FALSE)</f>
+        <v>0.42316363302800525</v>
+      </c>
+      <c r="H10" s="14" t="e">
+        <f>HLOOKUP('Sheet1 (2)'!$H$2,'Sheet1 (2)'!$N$3:$S$14,$D10,FALSE)</f>
+        <v>#N/A</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D11" s="14">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D11" s="11">
         <v>10</v>
       </c>
-      <c r="E11" s="18">
+      <c r="E11" s="14">
         <f>HLOOKUP(Sheet1!$H$2,Sheet1!$E$3:$J$14,$D11,FALSE)</f>
         <v>0.87287156094396945</v>
       </c>
-      <c r="F11" s="18">
-        <f>HLOOKUP(Sheet1!$H$2,Sheet1!$L$3:$Q$14,$D11,FALSE)</f>
-        <v>49.041666666666664</v>
+      <c r="F11" s="14">
+        <f>HLOOKUP(Sheet1!$H$2,Sheet1!$N$3:$S$14,$D11,FALSE)</f>
+        <v>181.77550256658165</v>
+      </c>
+      <c r="G11" s="14">
+        <f>HLOOKUP('Sheet1 (2)'!$H$2,'Sheet1 (2)'!$E$3:$J$14,$D11,FALSE)</f>
+        <v>0.34551165954032126</v>
+      </c>
+      <c r="H11" s="14" t="e">
+        <f>HLOOKUP('Sheet1 (2)'!$H$2,'Sheet1 (2)'!$N$3:$S$14,$D11,FALSE)</f>
+        <v>#N/A</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D12" s="14">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D12" s="11">
         <v>11</v>
       </c>
-      <c r="E12" s="18">
+      <c r="E12" s="14">
         <f>HLOOKUP(Sheet1!$H$2,Sheet1!$E$3:$J$14,$D12,FALSE)</f>
         <v>0.69631062382279141</v>
       </c>
-      <c r="F12" s="18">
-        <f>HLOOKUP(Sheet1!$H$2,Sheet1!$L$3:$Q$14,$D12,FALSE)</f>
-        <v>87.895833333333329</v>
+      <c r="F12" s="14">
+        <f>HLOOKUP(Sheet1!$H$2,Sheet1!$N$3:$S$14,$D12,FALSE)</f>
+        <v>361.90744673189579</v>
+      </c>
+      <c r="G12" s="14">
+        <f>HLOOKUP('Sheet1 (2)'!$H$2,'Sheet1 (2)'!$E$3:$J$14,$D12,FALSE)</f>
+        <v>0.27562295526318825</v>
+      </c>
+      <c r="H12" s="14" t="e">
+        <f>HLOOKUP('Sheet1 (2)'!$H$2,'Sheet1 (2)'!$N$3:$S$14,$D12,FALSE)</f>
+        <v>#N/A</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D13" s="14">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D13" s="11">
         <v>12</v>
       </c>
-      <c r="E13" s="18">
+      <c r="E13" s="14">
         <f>HLOOKUP(Sheet1!$H$2,Sheet1!$E$3:$J$14,$D13,FALSE)</f>
         <v>0.4747126632775413</v>
       </c>
-      <c r="F13" s="18">
-        <f>HLOOKUP(Sheet1!$H$2,Sheet1!$L$3:$Q$14,$D13,FALSE)</f>
-        <v>148.95833333333334</v>
+      <c r="F13" s="14">
+        <f>HLOOKUP(Sheet1!$H$2,Sheet1!$N$3:$S$14,$D13,FALSE)</f>
+        <v>840.50843987434189</v>
+      </c>
+      <c r="G13" s="14">
+        <f>HLOOKUP('Sheet1 (2)'!$H$2,'Sheet1 (2)'!$E$3:$J$14,$D13,FALSE)</f>
+        <v>0.18790709588069343</v>
+      </c>
+      <c r="H13" s="14" t="e">
+        <f>HLOOKUP('Sheet1 (2)'!$H$2,'Sheet1 (2)'!$N$3:$S$14,$D13,FALSE)</f>
+        <v>#N/A</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D15" s="20"/>
-      <c r="E15" s="20"/>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
     </row>
   </sheetData>
   <dataConsolidate/>
+  <mergeCells count="2">
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>

<commit_message>
pickaxe working as intended
</commit_message>
<xml_diff>
--- a/work_files/Pickaxe Power.xlsx
+++ b/work_files/Pickaxe Power.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="40">
   <si>
     <t>Pickaxe Power</t>
   </si>
@@ -113,9 +113,6 @@
     <t>Dirt</t>
   </si>
   <si>
-    <t>Can be buffed</t>
-  </si>
-  <si>
     <t>Red</t>
   </si>
   <si>
@@ -138,6 +135,12 @@
   </si>
   <si>
     <t>AtkPnt per swing</t>
+  </si>
+  <si>
+    <t>Actorvalue</t>
+  </si>
+  <si>
+    <t>Wut</t>
   </si>
 </sst>
 </file>
@@ -732,7 +735,7 @@
           <c:strCache>
             <c:ptCount val="1"/>
             <c:pt idx="0">
-              <c:v>Seconds take to break a stone tile</c:v>
+              <c:v>Seconds take to break a glass tile</c:v>
             </c:pt>
           </c:strCache>
         </c:strRef>
@@ -900,31 +903,31 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>0.41666666666666669</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.8284271247461898</c:v>
+                  <c:v>0.29462782549439476</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
+                  <c:v>0.20833333333333334</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.7888543819998317</c:v>
+                  <c:v>0.18633899812498247</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.3333333333333333</c:v>
+                  <c:v>0.1388888888888889</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.0690449676496976</c:v>
+                  <c:v>0.11135885079684349</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.87287156094396945</c:v>
+                  <c:v>9.0924120931663494E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.69631062382279141</c:v>
+                  <c:v>7.2532356648207438E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.4747126632775413</c:v>
+                  <c:v>4.944923575807722E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1122,7 +1125,7 @@
           <c:strCache>
             <c:ptCount val="1"/>
             <c:pt idx="0">
-              <c:v>Tool life for stone tiles</c:v>
+              <c:v>Tool life for glass tiles</c:v>
             </c:pt>
           </c:strCache>
         </c:strRef>
@@ -1279,31 +1282,31 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>12.25</c:v>
+                  <c:v>117.6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>41.247895569215274</c:v>
+                  <c:v>395.97979746446663</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>47.833333333333336</c:v>
+                  <c:v>459.2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>92.610482068116283</c:v>
+                  <c:v>889.06062785391634</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>79.75</c:v>
+                  <c:v>765.6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>188.95369803208402</c:v>
+                  <c:v>1813.955501108007</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>181.77550256658165</c:v>
+                  <c:v>1745.0448246391836</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>361.90744673189579</c:v>
+                  <c:v>3474.3114886261997</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>840.50843987434189</c:v>
+                  <c:v>8068.881022793681</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4004,7 +4007,7 @@
   <dimension ref="A1:S16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="A4" sqref="A4:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4030,7 +4033,7 @@
       </c>
       <c r="F2" s="12"/>
       <c r="H2" s="4" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L2" s="23" t="s">
         <v>37</v>
@@ -4044,7 +4047,7 @@
         <v>3</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="E3" s="17" t="s">
         <v>1</v>
@@ -4061,7 +4064,9 @@
       <c r="I3" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="J3" s="17"/>
+      <c r="J3" s="17" t="s">
+        <v>39</v>
+      </c>
       <c r="K3" s="17"/>
       <c r="L3" s="24"/>
       <c r="N3" s="17" t="str">
@@ -4084,9 +4089,9 @@
         <f>Table6[[#This Row],[Column5]]</f>
         <v>Metal</v>
       </c>
-      <c r="S3" s="17">
+      <c r="S3" s="17" t="str">
         <f>Table6[[#This Row],[Column6]]</f>
-        <v>0</v>
+        <v>Wut</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
@@ -4109,6 +4114,9 @@
       </c>
       <c r="I4">
         <v>125</v>
+      </c>
+      <c r="J4">
+        <v>-1</v>
       </c>
       <c r="L4" s="25"/>
     </row>
@@ -4134,10 +4142,10 @@
       <c r="J5" s="29"/>
       <c r="K5" s="18"/>
       <c r="L5" s="20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N5" s="30" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="O5" s="30"/>
       <c r="P5" s="30"/>
@@ -4178,11 +4186,11 @@
       </c>
       <c r="J6" s="2">
         <f>J$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B6))</f>
-        <v>0</v>
+        <v>-8.3333333333333329E-2</v>
       </c>
       <c r="L6" s="14">
         <f>4*SQRT(Table3[[#This Row],[ForceMod]])*VLOOKUP($L$2,Variables!$A$3:$B$4,2,FALSE)</f>
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="N6" s="14">
         <f>$C6/(E$4/(4*SQRT($B6)))</f>
@@ -4204,9 +4212,9 @@
         <f t="shared" si="0"/>
         <v>4.7039999999999997</v>
       </c>
-      <c r="S6" s="14" t="e">
+      <c r="S6" s="14">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>-588</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
@@ -4241,11 +4249,11 @@
       </c>
       <c r="J7" s="2">
         <f>J$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B7))</f>
-        <v>0</v>
+        <v>-5.8925565098878953E-2</v>
       </c>
       <c r="L7" s="14">
         <f>4*SQRT(Table3[[#This Row],[ForceMod]])*VLOOKUP($L$2,Variables!$A$3:$B$4,2,FALSE)</f>
-        <v>16.970562748477143</v>
+        <v>5.6568542494923806</v>
       </c>
       <c r="N7" s="14">
         <f t="shared" ref="N7:N14" si="1">$C7/(E$4/(4*SQRT($B7)))</f>
@@ -4267,9 +4275,9 @@
         <f t="shared" ref="R7:R14" si="5">$C7/(I$4/(4*SQRT($B7)))</f>
         <v>15.839191898578667</v>
       </c>
-      <c r="S7" s="14" t="e">
+      <c r="S7" s="14">
         <f t="shared" ref="S7:S14" si="6">$C7/(J$4/(4*SQRT($B7)))</f>
-        <v>#DIV/0!</v>
+        <v>-1979.8989873223331</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
@@ -4305,11 +4313,11 @@
       </c>
       <c r="J8" s="2">
         <f>J$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B8))</f>
-        <v>0</v>
+        <v>-4.1666666666666664E-2</v>
       </c>
       <c r="L8" s="14">
         <f>4*SQRT(Table3[[#This Row],[ForceMod]])*VLOOKUP($L$2,Variables!$A$3:$B$4,2,FALSE)</f>
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="N8" s="14">
         <f t="shared" si="1"/>
@@ -4331,9 +4339,9 @@
         <f t="shared" si="5"/>
         <v>18.367999999999999</v>
       </c>
-      <c r="S8" s="14" t="e">
+      <c r="S8" s="14">
         <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
+        <v>-2296</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
@@ -4369,11 +4377,11 @@
       </c>
       <c r="J9" s="2">
         <f>J$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B9))</f>
-        <v>0</v>
+        <v>-3.7267799624996496E-2</v>
       </c>
       <c r="L9" s="14">
         <f>4*SQRT(Table3[[#This Row],[ForceMod]])*VLOOKUP($L$2,Variables!$A$3:$B$4,2,FALSE)</f>
-        <v>26.832815729997478</v>
+        <v>8.9442719099991592</v>
       </c>
       <c r="N9" s="14">
         <f t="shared" si="1"/>
@@ -4395,9 +4403,9 @@
         <f t="shared" si="5"/>
         <v>35.562425114156653</v>
       </c>
-      <c r="S9" s="14" t="e">
+      <c r="S9" s="14">
         <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
+        <v>-4445.3031392695821</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
@@ -4433,11 +4441,11 @@
       </c>
       <c r="J10" s="2">
         <f>J$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B10))</f>
-        <v>0</v>
+        <v>-2.7777777777777776E-2</v>
       </c>
       <c r="L10" s="14">
         <f>4*SQRT(Table3[[#This Row],[ForceMod]])*VLOOKUP($L$2,Variables!$A$3:$B$4,2,FALSE)</f>
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="N10" s="14">
         <f t="shared" si="1"/>
@@ -4459,9 +4467,9 @@
         <f t="shared" si="5"/>
         <v>30.624000000000002</v>
       </c>
-      <c r="S10" s="14" t="e">
+      <c r="S10" s="14">
         <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
+        <v>-3828</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
@@ -4497,11 +4505,11 @@
       </c>
       <c r="J11" s="2">
         <f>J$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B11))</f>
-        <v>0</v>
+        <v>-2.2271770159368699E-2</v>
       </c>
       <c r="L11" s="14">
         <f>4*SQRT(Table3[[#This Row],[ForceMod]])*VLOOKUP($L$2,Variables!$A$3:$B$4,2,FALSE)</f>
-        <v>44.899888641287298</v>
+        <v>14.966629547095765</v>
       </c>
       <c r="N11" s="14">
         <f t="shared" si="1"/>
@@ -4523,9 +4531,9 @@
         <f t="shared" si="5"/>
         <v>72.558220044320265</v>
       </c>
-      <c r="S11" s="14" t="e">
+      <c r="S11" s="14">
         <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
+        <v>-9069.7775055400343</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
@@ -4561,11 +4569,11 @@
       </c>
       <c r="J12" s="2">
         <f>J$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B12))</f>
-        <v>0</v>
+        <v>-1.8184824186332698E-2</v>
       </c>
       <c r="L12" s="14">
         <f>4*SQRT(Table3[[#This Row],[ForceMod]])*VLOOKUP($L$2,Variables!$A$3:$B$4,2,FALSE)</f>
-        <v>54.990908339470082</v>
+        <v>18.330302779823359</v>
       </c>
       <c r="N12" s="14">
         <f t="shared" si="1"/>
@@ -4587,9 +4595,9 @@
         <f t="shared" si="5"/>
         <v>69.801792985567346</v>
       </c>
-      <c r="S12" s="14" t="e">
+      <c r="S12" s="14">
         <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
+        <v>-8725.2241231959197</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
@@ -4625,11 +4633,11 @@
       </c>
       <c r="J13" s="2">
         <f>J$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B13))</f>
-        <v>0</v>
+        <v>-1.4506471329641486E-2</v>
       </c>
       <c r="L13" s="14">
         <f>4*SQRT(Table3[[#This Row],[ForceMod]])*VLOOKUP($L$2,Variables!$A$3:$B$4,2,FALSE)</f>
-        <v>68.934751758456343</v>
+        <v>22.978250586152114</v>
       </c>
       <c r="N13" s="14">
         <f t="shared" si="1"/>
@@ -4651,9 +4659,9 @@
         <f t="shared" si="5"/>
         <v>138.97245954504797</v>
       </c>
-      <c r="S13" s="14" t="e">
+      <c r="S13" s="14">
         <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
+        <v>-17371.557443130998</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
@@ -4689,11 +4697,11 @@
       </c>
       <c r="J14" s="2">
         <f>J$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B14))</f>
-        <v>0</v>
+        <v>-9.8898471516154444E-3</v>
       </c>
       <c r="L14" s="14">
         <f>4*SQRT(Table3[[#This Row],[ForceMod]])*VLOOKUP($L$2,Variables!$A$3:$B$4,2,FALSE)</f>
-        <v>101.11379727811631</v>
+        <v>33.704599092705436</v>
       </c>
       <c r="N14" s="14">
         <f t="shared" si="1"/>
@@ -4715,9 +4723,9 @@
         <f t="shared" si="5"/>
         <v>322.75524091174725</v>
       </c>
-      <c r="S14" s="14" t="e">
+      <c r="S14" s="14">
         <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
+        <v>-40344.405113968409</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
@@ -4836,7 +4844,7 @@
         <v>16</v>
       </c>
       <c r="F3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G3" s="17" t="s">
         <v>15</v>
@@ -4910,7 +4918,7 @@
       <c r="I5" s="29"/>
       <c r="J5" s="29"/>
       <c r="L5" s="30" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M5" s="30"/>
       <c r="N5" s="30"/>
@@ -5553,11 +5561,11 @@
       </c>
       <c r="D1" s="11" t="str">
         <f>Sheet1!E2&amp;" to break a "&amp;LOWER(Sheet1!H2)&amp;" tile"</f>
-        <v>Seconds take to break a stone tile</v>
+        <v>Seconds take to break a glass tile</v>
       </c>
       <c r="E1" s="11" t="str">
         <f>"Tool life for "&amp;LOWER(Sheet1!H2)&amp;" tiles"</f>
-        <v>Tool life for stone tiles</v>
+        <v>Tool life for glass tiles</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -5578,30 +5586,30 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B3" s="10">
         <f>Sheet1!B3</f>
         <v>3</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F3" s="15"/>
       <c r="G3" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H3" s="15"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E4" s="16" t="s">
         <v>27</v>
@@ -5622,11 +5630,11 @@
       </c>
       <c r="E5" s="14">
         <f>HLOOKUP(Sheet1!$H$2,Sheet1!$E$3:$J$14,$D5,FALSE)</f>
-        <v>4</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="F5" s="14">
         <f>HLOOKUP(Sheet1!$H$2,Sheet1!$N$3:$S$14,$D5,FALSE)</f>
-        <v>12.25</v>
+        <v>117.6</v>
       </c>
       <c r="G5" s="14">
         <f>HLOOKUP('Sheet1 (2)'!$H$2,'Sheet1 (2)'!$E$3:$J$14,$D5,FALSE)</f>
@@ -5643,11 +5651,11 @@
       </c>
       <c r="E6" s="14">
         <f>HLOOKUP(Sheet1!$H$2,Sheet1!$E$3:$J$14,$D6,FALSE)</f>
-        <v>2.8284271247461898</v>
+        <v>0.29462782549439476</v>
       </c>
       <c r="F6" s="14">
         <f>HLOOKUP(Sheet1!$H$2,Sheet1!$N$3:$S$14,$D6,FALSE)</f>
-        <v>41.247895569215274</v>
+        <v>395.97979746446663</v>
       </c>
       <c r="G6" s="14">
         <f>HLOOKUP('Sheet1 (2)'!$H$2,'Sheet1 (2)'!$E$3:$J$14,$D6,FALSE)</f>
@@ -5664,11 +5672,11 @@
       </c>
       <c r="E7" s="14">
         <f>HLOOKUP(Sheet1!$H$2,Sheet1!$E$3:$J$14,$D7,FALSE)</f>
-        <v>2</v>
+        <v>0.20833333333333334</v>
       </c>
       <c r="F7" s="14">
         <f>HLOOKUP(Sheet1!$H$2,Sheet1!$N$3:$S$14,$D7,FALSE)</f>
-        <v>47.833333333333336</v>
+        <v>459.2</v>
       </c>
       <c r="G7" s="14">
         <f>HLOOKUP('Sheet1 (2)'!$H$2,'Sheet1 (2)'!$E$3:$J$14,$D7,FALSE)</f>
@@ -5685,11 +5693,11 @@
       </c>
       <c r="E8" s="14">
         <f>HLOOKUP(Sheet1!$H$2,Sheet1!$E$3:$J$14,$D8,FALSE)</f>
-        <v>1.7888543819998317</v>
+        <v>0.18633899812498247</v>
       </c>
       <c r="F8" s="14">
         <f>HLOOKUP(Sheet1!$H$2,Sheet1!$N$3:$S$14,$D8,FALSE)</f>
-        <v>92.610482068116283</v>
+        <v>889.06062785391634</v>
       </c>
       <c r="G8" s="14">
         <f>HLOOKUP('Sheet1 (2)'!$H$2,'Sheet1 (2)'!$E$3:$J$14,$D8,FALSE)</f>
@@ -5706,11 +5714,11 @@
       </c>
       <c r="E9" s="14">
         <f>HLOOKUP(Sheet1!$H$2,Sheet1!$E$3:$J$14,$D9,FALSE)</f>
-        <v>1.3333333333333333</v>
+        <v>0.1388888888888889</v>
       </c>
       <c r="F9" s="14">
         <f>HLOOKUP(Sheet1!$H$2,Sheet1!$N$3:$S$14,$D9,FALSE)</f>
-        <v>79.75</v>
+        <v>765.6</v>
       </c>
       <c r="G9" s="14">
         <f>HLOOKUP('Sheet1 (2)'!$H$2,'Sheet1 (2)'!$E$3:$J$14,$D9,FALSE)</f>
@@ -5727,11 +5735,11 @@
       </c>
       <c r="E10" s="14">
         <f>HLOOKUP(Sheet1!$H$2,Sheet1!$E$3:$J$14,$D10,FALSE)</f>
-        <v>1.0690449676496976</v>
+        <v>0.11135885079684349</v>
       </c>
       <c r="F10" s="14">
         <f>HLOOKUP(Sheet1!$H$2,Sheet1!$N$3:$S$14,$D10,FALSE)</f>
-        <v>188.95369803208402</v>
+        <v>1813.955501108007</v>
       </c>
       <c r="G10" s="14">
         <f>HLOOKUP('Sheet1 (2)'!$H$2,'Sheet1 (2)'!$E$3:$J$14,$D10,FALSE)</f>
@@ -5748,11 +5756,11 @@
       </c>
       <c r="E11" s="14">
         <f>HLOOKUP(Sheet1!$H$2,Sheet1!$E$3:$J$14,$D11,FALSE)</f>
-        <v>0.87287156094396945</v>
+        <v>9.0924120931663494E-2</v>
       </c>
       <c r="F11" s="14">
         <f>HLOOKUP(Sheet1!$H$2,Sheet1!$N$3:$S$14,$D11,FALSE)</f>
-        <v>181.77550256658165</v>
+        <v>1745.0448246391836</v>
       </c>
       <c r="G11" s="14">
         <f>HLOOKUP('Sheet1 (2)'!$H$2,'Sheet1 (2)'!$E$3:$J$14,$D11,FALSE)</f>
@@ -5769,11 +5777,11 @@
       </c>
       <c r="E12" s="14">
         <f>HLOOKUP(Sheet1!$H$2,Sheet1!$E$3:$J$14,$D12,FALSE)</f>
-        <v>0.69631062382279141</v>
+        <v>7.2532356648207438E-2</v>
       </c>
       <c r="F12" s="14">
         <f>HLOOKUP(Sheet1!$H$2,Sheet1!$N$3:$S$14,$D12,FALSE)</f>
-        <v>361.90744673189579</v>
+        <v>3474.3114886261997</v>
       </c>
       <c r="G12" s="14">
         <f>HLOOKUP('Sheet1 (2)'!$H$2,'Sheet1 (2)'!$E$3:$J$14,$D12,FALSE)</f>
@@ -5790,11 +5798,11 @@
       </c>
       <c r="E13" s="14">
         <f>HLOOKUP(Sheet1!$H$2,Sheet1!$E$3:$J$14,$D13,FALSE)</f>
-        <v>0.4747126632775413</v>
+        <v>4.944923575807722E-2</v>
       </c>
       <c r="F13" s="14">
         <f>HLOOKUP(Sheet1!$H$2,Sheet1!$N$3:$S$14,$D13,FALSE)</f>
-        <v>840.50843987434189</v>
+        <v>8068.881022793681</v>
       </c>
       <c r="G13" s="14">
         <f>HLOOKUP('Sheet1 (2)'!$H$2,'Sheet1 (2)'!$E$3:$J$14,$D13,FALSE)</f>

</xml_diff>

<commit_message>
Resolving issue #18 and #19
</commit_message>
<xml_diff>
--- a/work_files/Pickaxe Power.xlsx
+++ b/work_files/Pickaxe Power.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="43">
   <si>
     <t>Pickaxe Power</t>
   </si>
@@ -142,17 +142,33 @@
   <si>
     <t>Wut</t>
   </si>
+  <si>
+    <t>to break</t>
+  </si>
+  <si>
+    <t>tile</t>
+  </si>
+  <si>
+    <t>Query:</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -251,8 +267,23 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="0" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -281,8 +312,19 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -394,77 +436,251 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="8">
+  <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="3" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="5"/>
-    <xf numFmtId="2" fontId="9" fillId="3" borderId="3" xfId="5" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="4" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="5"/>
+    <xf numFmtId="2" fontId="10" fillId="3" borderId="3" xfId="5" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="3" xfId="6"/>
+    <xf numFmtId="2" fontId="4" fillId="2" borderId="1" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="8" xfId="5" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="7" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="5"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="3" borderId="5" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="3" borderId="6" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="3" borderId="7" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="3" xfId="6"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="5"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="2" borderId="1" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="11" xfId="5" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="11" xfId="5" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="10" xfId="9" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="12" xfId="9" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="9" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="10" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="10" fillId="3" borderId="5" xfId="5" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="18" xfId="6" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="18" xfId="5" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="19" xfId="5" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="20" xfId="6" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="13" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="14" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="3" applyFont="1"/>
-    <xf numFmtId="49" fontId="13" fillId="3" borderId="5" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="3" borderId="6" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="3" borderId="7" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="8" xfId="5" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="7" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="15" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="2" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="8">
+  <cellStyles count="10">
     <cellStyle name="20% - Accent3" xfId="7" builtinId="38"/>
+    <cellStyle name="40% - Accent3" xfId="9" builtinId="39"/>
+    <cellStyle name="Accent3" xfId="8" builtinId="37"/>
     <cellStyle name="Calculation" xfId="6" builtinId="22"/>
     <cellStyle name="Explanatory Text" xfId="3" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="4" builtinId="19"/>
@@ -473,7 +689,45 @@
     <cellStyle name="Output" xfId="2" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="14">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor theme="0" tint="-0.14999847407452621"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="2" tint="-0.749992370372631"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -570,44 +824,7 @@
       </fill>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="2" tint="-0.749992370372631"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
@@ -620,29 +837,6 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor theme="0" tint="-0.14999847407452621"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
@@ -735,7 +929,7 @@
           <c:strCache>
             <c:ptCount val="1"/>
             <c:pt idx="0">
-              <c:v>Seconds take to break a glass tile</c:v>
+              <c:v>Seconds take to break a stone tile</c:v>
             </c:pt>
           </c:strCache>
         </c:strRef>
@@ -903,31 +1097,31 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>0.41666666666666669</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.29462782549439476</c:v>
+                  <c:v>2.8284271247461898</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.20833333333333334</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.18633899812498247</c:v>
+                  <c:v>1.7888543819998317</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.1388888888888889</c:v>
+                  <c:v>1.3333333333333333</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.11135885079684349</c:v>
+                  <c:v>1.0690449676496976</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9.0924120931663494E-2</c:v>
+                  <c:v>0.87287156094396945</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7.2532356648207438E-2</c:v>
+                  <c:v>0.69631062382279141</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.944923575807722E-2</c:v>
+                  <c:v>0.4747126632775413</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1125,7 +1319,7 @@
           <c:strCache>
             <c:ptCount val="1"/>
             <c:pt idx="0">
-              <c:v>Tool life for glass tiles</c:v>
+              <c:v>Tool life for stone tiles</c:v>
             </c:pt>
           </c:strCache>
         </c:strRef>
@@ -1282,31 +1476,31 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>117.6</c:v>
+                  <c:v>12.25</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>395.97979746446663</c:v>
+                  <c:v>41.247895569215274</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>459.2</c:v>
+                  <c:v>47.833333333333336</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>889.06062785391634</c:v>
+                  <c:v>92.610482068116283</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>765.6</c:v>
+                  <c:v>79.75</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1813.955501108007</c:v>
+                  <c:v>188.95369803208402</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1745.0448246391836</c:v>
+                  <c:v>181.77550256658165</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3474.3114886261997</c:v>
+                  <c:v>361.90744673189579</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8068.881022793681</c:v>
+                  <c:v>840.50843987434189</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3670,15 +3864,15 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A5:C14" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13" tableBorderDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A5:C14" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12" tableBorderDxfId="11">
   <autoFilter ref="A5:C14"/>
   <sortState ref="A6:B14">
     <sortCondition ref="B5:B14"/>
   </sortState>
   <tableColumns count="3">
-    <tableColumn id="1" name="Material" dataDxfId="6" dataCellStyle="20% - Accent3"/>
+    <tableColumn id="1" name="Material" dataCellStyle="20% - Accent3"/>
     <tableColumn id="2" name="ForceMod" dataCellStyle="Input"/>
-    <tableColumn id="4" name="Durability" dataDxfId="11"/>
+    <tableColumn id="4" name="Durability" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="1" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -3690,7 +3884,7 @@
     <filterColumn colId="0" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="1">
-    <tableColumn id="1" name="AtkPoint" dataDxfId="7" dataCellStyle="Output">
+    <tableColumn id="1" name="AtkPoint" dataDxfId="8" dataCellStyle="Output">
       <calculatedColumnFormula>4*SQRT(Table3[[#This Row],[ForceMod]])*VLOOKUP($L$2,Variables!$A$3:$B$4,2,FALSE)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3713,17 +3907,19 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table35" displayName="Table35" ref="A5:C14" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4" tableBorderDxfId="3" dataCellStyle="Output">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table35" displayName="Table35" ref="A5:C14" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6" tableBorderDxfId="5" dataCellStyle="Output">
   <autoFilter ref="A5:C14"/>
   <sortState ref="A6:B14">
     <sortCondition ref="B5:B14"/>
   </sortState>
   <tableColumns count="3">
-    <tableColumn id="1" name="Material" dataDxfId="2" dataCellStyle="Output"/>
-    <tableColumn id="2" name="ForceMod" dataDxfId="1" dataCellStyle="Output">
+    <tableColumn id="1" name="Material" dataDxfId="4" dataCellStyle="Output">
+      <calculatedColumnFormula>Table3[[#This Row],[Material]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="2" name="ForceMod" dataDxfId="3" dataCellStyle="Output">
       <calculatedColumnFormula>Table3[[#This Row],[ForceMod]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Durability" dataDxfId="0" dataCellStyle="Output">
+    <tableColumn id="3" name="Durability" dataDxfId="2" dataCellStyle="Output">
       <calculatedColumnFormula>Table3[[#This Row],[Durability]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3734,7 +3930,7 @@
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table7" displayName="Table7" ref="A1:B4" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="2">
-    <tableColumn id="1" name="Name" dataDxfId="8"/>
+    <tableColumn id="1" name="Name" dataDxfId="1"/>
     <tableColumn id="2" name="Value"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -4007,7 +4203,7 @@
   <dimension ref="A1:S16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:C4"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4028,14 +4224,24 @@
       </c>
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E2" s="12" t="s">
+      <c r="C2" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="37"/>
+      <c r="E2" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="12"/>
-      <c r="H2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="L2" s="23" t="s">
+      <c r="F2" s="32"/>
+      <c r="G2" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="H2" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="L2" s="27" t="s">
         <v>37</v>
       </c>
     </row>
@@ -4043,63 +4249,63 @@
       <c r="A3" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="38">
         <v>3</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="E3" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="17" t="s">
+      <c r="F3" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="17" t="s">
+      <c r="G3" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="H3" s="17" t="s">
+      <c r="H3" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="17" t="s">
+      <c r="I3" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="J3" s="17" t="s">
+      <c r="J3" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="K3" s="17"/>
-      <c r="L3" s="24"/>
-      <c r="N3" s="17" t="str">
+      <c r="K3" s="13"/>
+      <c r="L3" s="28"/>
+      <c r="N3" s="13" t="str">
         <f>Table6[[#This Row],[Column1]]</f>
         <v>Stone</v>
       </c>
-      <c r="O3" s="17" t="str">
+      <c r="O3" s="13" t="str">
         <f>Table6[[#This Row],[Column2]]</f>
         <v>Ice</v>
       </c>
-      <c r="P3" s="17" t="str">
+      <c r="P3" s="13" t="str">
         <f>Table6[[#This Row],[Column3]]</f>
         <v>Dirt</v>
       </c>
-      <c r="Q3" s="17" t="str">
+      <c r="Q3" s="13" t="str">
         <f>Table6[[#This Row],[Column4]]</f>
         <v>Glass</v>
       </c>
-      <c r="R3" s="17" t="str">
+      <c r="R3" s="13" t="str">
         <f>Table6[[#This Row],[Column5]]</f>
         <v>Metal</v>
       </c>
-      <c r="S3" s="17" t="str">
+      <c r="S3" s="13" t="str">
         <f>Table6[[#This Row],[Column6]]</f>
         <v>Wut</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
+      <c r="B4" s="46"/>
+      <c r="C4" s="47"/>
       <c r="E4">
         <v>48</v>
       </c>
@@ -4118,49 +4324,49 @@
       <c r="J4">
         <v>-1</v>
       </c>
-      <c r="L4" s="25"/>
+      <c r="L4" s="29"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="39" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="26"/>
-      <c r="E5" s="29" t="str">
+      <c r="D5" s="18"/>
+      <c r="E5" s="23" t="str">
         <f>E2&amp;" to take one tile"</f>
         <v>Seconds take to take one tile</v>
       </c>
-      <c r="F5" s="29"/>
-      <c r="G5" s="29"/>
-      <c r="H5" s="29"/>
-      <c r="I5" s="29"/>
-      <c r="J5" s="29"/>
-      <c r="K5" s="18"/>
-      <c r="L5" s="20" t="s">
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="23"/>
+      <c r="I5" s="23"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="N5" s="30" t="s">
+      <c r="N5" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="O5" s="30"/>
-      <c r="P5" s="30"/>
-      <c r="Q5" s="30"/>
-      <c r="R5" s="30"/>
-      <c r="S5" s="30"/>
+      <c r="O5" s="25"/>
+      <c r="P5" s="25"/>
+      <c r="Q5" s="25"/>
+      <c r="R5" s="25"/>
+      <c r="S5" s="25"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" s="28" t="s">
+      <c r="A6" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="27">
+      <c r="B6" s="19">
         <v>1</v>
       </c>
-      <c r="C6" s="11">
+      <c r="C6" s="41">
         <f>ROUND(0.42*C7,0)</f>
         <v>147</v>
       </c>
@@ -4188,43 +4394,43 @@
         <f>J$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B6))</f>
         <v>-8.3333333333333329E-2</v>
       </c>
-      <c r="L6" s="14">
+      <c r="L6" s="11">
         <f>4*SQRT(Table3[[#This Row],[ForceMod]])*VLOOKUP($L$2,Variables!$A$3:$B$4,2,FALSE)</f>
         <v>4</v>
       </c>
-      <c r="N6" s="14">
+      <c r="N6" s="11">
         <f>$C6/(E$4/(4*SQRT($B6)))</f>
         <v>12.25</v>
       </c>
-      <c r="O6" s="14">
+      <c r="O6" s="11">
         <f t="shared" ref="O6:S6" si="0">$C6/(F$4/(4*SQRT($B6)))</f>
         <v>16.8</v>
       </c>
-      <c r="P6" s="14">
+      <c r="P6" s="11">
         <f t="shared" si="0"/>
         <v>24.5</v>
       </c>
-      <c r="Q6" s="14">
+      <c r="Q6" s="11">
         <f t="shared" si="0"/>
         <v>117.6</v>
       </c>
-      <c r="R6" s="14">
+      <c r="R6" s="11">
         <f t="shared" si="0"/>
         <v>4.7039999999999997</v>
       </c>
-      <c r="S6" s="14">
+      <c r="S6" s="11">
         <f t="shared" si="0"/>
         <v>-588</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7" s="28" t="s">
+      <c r="A7" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="27">
+      <c r="B7" s="19">
         <v>2</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="42">
         <v>350</v>
       </c>
       <c r="E7" s="2">
@@ -4251,43 +4457,43 @@
         <f>J$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B7))</f>
         <v>-5.8925565098878953E-2</v>
       </c>
-      <c r="L7" s="14">
+      <c r="L7" s="11">
         <f>4*SQRT(Table3[[#This Row],[ForceMod]])*VLOOKUP($L$2,Variables!$A$3:$B$4,2,FALSE)</f>
         <v>5.6568542494923806</v>
       </c>
-      <c r="N7" s="14">
+      <c r="N7" s="11">
         <f t="shared" ref="N7:N14" si="1">$C7/(E$4/(4*SQRT($B7)))</f>
         <v>41.247895569215274</v>
       </c>
-      <c r="O7" s="14">
+      <c r="O7" s="11">
         <f t="shared" ref="O7:O14" si="2">$C7/(F$4/(4*SQRT($B7)))</f>
         <v>56.568542494923811</v>
       </c>
-      <c r="P7" s="14">
+      <c r="P7" s="11">
         <f t="shared" ref="P7:P14" si="3">$C7/(G$4/(4*SQRT($B7)))</f>
         <v>82.495791138430548</v>
       </c>
-      <c r="Q7" s="14">
+      <c r="Q7" s="11">
         <f t="shared" ref="Q7:Q14" si="4">$C7/(H$4/(4*SQRT($B7)))</f>
         <v>395.97979746446663</v>
       </c>
-      <c r="R7" s="14">
+      <c r="R7" s="11">
         <f t="shared" ref="R7:R14" si="5">$C7/(I$4/(4*SQRT($B7)))</f>
         <v>15.839191898578667</v>
       </c>
-      <c r="S7" s="14">
+      <c r="S7" s="11">
         <f t="shared" ref="S7:S14" si="6">$C7/(J$4/(4*SQRT($B7)))</f>
         <v>-1979.8989873223331</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A8" s="28" t="s">
+      <c r="A8" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="27">
+      <c r="B8" s="19">
         <v>4</v>
       </c>
-      <c r="C8" s="11">
+      <c r="C8" s="41">
         <f>ROUND(0.82*C7,0)</f>
         <v>287</v>
       </c>
@@ -4315,43 +4521,43 @@
         <f>J$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B8))</f>
         <v>-4.1666666666666664E-2</v>
       </c>
-      <c r="L8" s="14">
+      <c r="L8" s="11">
         <f>4*SQRT(Table3[[#This Row],[ForceMod]])*VLOOKUP($L$2,Variables!$A$3:$B$4,2,FALSE)</f>
         <v>8</v>
       </c>
-      <c r="N8" s="14">
+      <c r="N8" s="11">
         <f t="shared" si="1"/>
         <v>47.833333333333336</v>
       </c>
-      <c r="O8" s="14">
+      <c r="O8" s="11">
         <f t="shared" si="2"/>
         <v>65.599999999999994</v>
       </c>
-      <c r="P8" s="14">
+      <c r="P8" s="11">
         <f t="shared" si="3"/>
         <v>95.666666666666671</v>
       </c>
-      <c r="Q8" s="14">
+      <c r="Q8" s="11">
         <f t="shared" si="4"/>
         <v>459.2</v>
       </c>
-      <c r="R8" s="14">
+      <c r="R8" s="11">
         <f t="shared" si="5"/>
         <v>18.367999999999999</v>
       </c>
-      <c r="S8" s="14">
+      <c r="S8" s="11">
         <f t="shared" si="6"/>
         <v>-2296</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" s="28" t="s">
+      <c r="A9" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="27">
+      <c r="B9" s="19">
         <v>5</v>
       </c>
-      <c r="C9" s="11">
+      <c r="C9" s="41">
         <f>ROUND(1.42*C7,0)</f>
         <v>497</v>
       </c>
@@ -4379,43 +4585,43 @@
         <f>J$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B9))</f>
         <v>-3.7267799624996496E-2</v>
       </c>
-      <c r="L9" s="14">
+      <c r="L9" s="11">
         <f>4*SQRT(Table3[[#This Row],[ForceMod]])*VLOOKUP($L$2,Variables!$A$3:$B$4,2,FALSE)</f>
         <v>8.9442719099991592</v>
       </c>
-      <c r="N9" s="14">
+      <c r="N9" s="11">
         <f t="shared" si="1"/>
         <v>92.610482068116283</v>
       </c>
-      <c r="O9" s="14">
+      <c r="O9" s="11">
         <f t="shared" si="2"/>
         <v>127.00866112198807</v>
       </c>
-      <c r="P9" s="14">
+      <c r="P9" s="11">
         <f t="shared" si="3"/>
         <v>185.22096413623257</v>
       </c>
-      <c r="Q9" s="14">
+      <c r="Q9" s="11">
         <f t="shared" si="4"/>
         <v>889.06062785391634</v>
       </c>
-      <c r="R9" s="14">
+      <c r="R9" s="11">
         <f t="shared" si="5"/>
         <v>35.562425114156653</v>
       </c>
-      <c r="S9" s="14">
+      <c r="S9" s="11">
         <f t="shared" si="6"/>
         <v>-4445.3031392695821</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" s="28" t="s">
+      <c r="A10" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="27">
+      <c r="B10" s="19">
         <v>9</v>
       </c>
-      <c r="C10" s="11">
+      <c r="C10" s="41">
         <f>ROUND(0.91*C7,0)</f>
         <v>319</v>
       </c>
@@ -4443,43 +4649,43 @@
         <f>J$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B10))</f>
         <v>-2.7777777777777776E-2</v>
       </c>
-      <c r="L10" s="14">
+      <c r="L10" s="11">
         <f>4*SQRT(Table3[[#This Row],[ForceMod]])*VLOOKUP($L$2,Variables!$A$3:$B$4,2,FALSE)</f>
         <v>12</v>
       </c>
-      <c r="N10" s="14">
+      <c r="N10" s="11">
         <f t="shared" si="1"/>
         <v>79.75</v>
       </c>
-      <c r="O10" s="14">
+      <c r="O10" s="11">
         <f t="shared" si="2"/>
         <v>109.37142857142858</v>
       </c>
-      <c r="P10" s="14">
+      <c r="P10" s="11">
         <f t="shared" si="3"/>
         <v>159.5</v>
       </c>
-      <c r="Q10" s="14">
+      <c r="Q10" s="11">
         <f t="shared" si="4"/>
         <v>765.6</v>
       </c>
-      <c r="R10" s="14">
+      <c r="R10" s="11">
         <f t="shared" si="5"/>
         <v>30.624000000000002</v>
       </c>
-      <c r="S10" s="14">
+      <c r="S10" s="11">
         <f t="shared" si="6"/>
         <v>-3828</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="28" t="s">
+      <c r="A11" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="27">
+      <c r="B11" s="19">
         <v>14</v>
       </c>
-      <c r="C11" s="11">
+      <c r="C11" s="41">
         <f>ROUND(1.73*C7,0)</f>
         <v>606</v>
       </c>
@@ -4507,43 +4713,43 @@
         <f>J$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B11))</f>
         <v>-2.2271770159368699E-2</v>
       </c>
-      <c r="L11" s="14">
+      <c r="L11" s="11">
         <f>4*SQRT(Table3[[#This Row],[ForceMod]])*VLOOKUP($L$2,Variables!$A$3:$B$4,2,FALSE)</f>
         <v>14.966629547095765</v>
       </c>
-      <c r="N11" s="14">
+      <c r="N11" s="11">
         <f t="shared" si="1"/>
         <v>188.95369803208402</v>
       </c>
-      <c r="O11" s="14">
+      <c r="O11" s="11">
         <f t="shared" si="2"/>
         <v>259.13650015828665</v>
       </c>
-      <c r="P11" s="14">
+      <c r="P11" s="11">
         <f t="shared" si="3"/>
         <v>377.90739606416804</v>
       </c>
-      <c r="Q11" s="14">
+      <c r="Q11" s="11">
         <f t="shared" si="4"/>
         <v>1813.955501108007</v>
       </c>
-      <c r="R11" s="14">
+      <c r="R11" s="11">
         <f t="shared" si="5"/>
         <v>72.558220044320265</v>
       </c>
-      <c r="S11" s="14">
+      <c r="S11" s="11">
         <f t="shared" si="6"/>
         <v>-9069.7775055400343</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" s="28" t="s">
+      <c r="A12" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="27">
+      <c r="B12" s="19">
         <v>21</v>
       </c>
-      <c r="C12" s="11">
+      <c r="C12" s="41">
         <f>ROUND(1.36*C7,0)</f>
         <v>476</v>
       </c>
@@ -4571,43 +4777,43 @@
         <f>J$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B12))</f>
         <v>-1.8184824186332698E-2</v>
       </c>
-      <c r="L12" s="14">
+      <c r="L12" s="11">
         <f>4*SQRT(Table3[[#This Row],[ForceMod]])*VLOOKUP($L$2,Variables!$A$3:$B$4,2,FALSE)</f>
         <v>18.330302779823359</v>
       </c>
-      <c r="N12" s="14">
+      <c r="N12" s="11">
         <f t="shared" si="1"/>
         <v>181.77550256658165</v>
       </c>
-      <c r="O12" s="14">
+      <c r="O12" s="11">
         <f t="shared" si="2"/>
         <v>249.29211780559768</v>
       </c>
-      <c r="P12" s="14">
+      <c r="P12" s="11">
         <f t="shared" si="3"/>
         <v>363.5510051331633</v>
       </c>
-      <c r="Q12" s="14">
+      <c r="Q12" s="11">
         <f t="shared" si="4"/>
         <v>1745.0448246391836</v>
       </c>
-      <c r="R12" s="14">
+      <c r="R12" s="11">
         <f t="shared" si="5"/>
         <v>69.801792985567346</v>
       </c>
-      <c r="S12" s="14">
+      <c r="S12" s="11">
         <f t="shared" si="6"/>
         <v>-8725.2241231959197</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A13" s="28" t="s">
+      <c r="A13" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="27">
+      <c r="B13" s="19">
         <v>33</v>
       </c>
-      <c r="C13" s="11">
+      <c r="C13" s="41">
         <f>ROUND(2.16*C7,0)</f>
         <v>756</v>
       </c>
@@ -4635,43 +4841,43 @@
         <f>J$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B13))</f>
         <v>-1.4506471329641486E-2</v>
       </c>
-      <c r="L13" s="14">
+      <c r="L13" s="11">
         <f>4*SQRT(Table3[[#This Row],[ForceMod]])*VLOOKUP($L$2,Variables!$A$3:$B$4,2,FALSE)</f>
         <v>22.978250586152114</v>
       </c>
-      <c r="N13" s="14">
+      <c r="N13" s="11">
         <f t="shared" si="1"/>
         <v>361.90744673189579</v>
       </c>
-      <c r="O13" s="14">
+      <c r="O13" s="11">
         <f t="shared" si="2"/>
         <v>496.33021266088571</v>
       </c>
-      <c r="P13" s="14">
+      <c r="P13" s="11">
         <f t="shared" si="3"/>
         <v>723.81489346379158</v>
       </c>
-      <c r="Q13" s="14">
+      <c r="Q13" s="11">
         <f t="shared" si="4"/>
         <v>3474.3114886261997</v>
       </c>
-      <c r="R13" s="14">
+      <c r="R13" s="11">
         <f t="shared" si="5"/>
         <v>138.97245954504797</v>
       </c>
-      <c r="S13" s="14">
+      <c r="S13" s="11">
         <f t="shared" si="6"/>
         <v>-17371.557443130998</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A14" s="28" t="s">
+      <c r="A14" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="27">
+      <c r="B14" s="43">
         <v>71</v>
       </c>
-      <c r="C14" s="11">
+      <c r="C14" s="44">
         <f>ROUND(3.42*C7,0)</f>
         <v>1197</v>
       </c>
@@ -4699,31 +4905,31 @@
         <f>J$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B14))</f>
         <v>-9.8898471516154444E-3</v>
       </c>
-      <c r="L14" s="14">
+      <c r="L14" s="11">
         <f>4*SQRT(Table3[[#This Row],[ForceMod]])*VLOOKUP($L$2,Variables!$A$3:$B$4,2,FALSE)</f>
         <v>33.704599092705436</v>
       </c>
-      <c r="N14" s="14">
+      <c r="N14" s="11">
         <f t="shared" si="1"/>
         <v>840.50843987434189</v>
       </c>
-      <c r="O14" s="14">
+      <c r="O14" s="11">
         <f t="shared" si="2"/>
         <v>1152.697288970526</v>
       </c>
-      <c r="P14" s="14">
+      <c r="P14" s="11">
         <f t="shared" si="3"/>
         <v>1681.0168797486838</v>
       </c>
-      <c r="Q14" s="14">
+      <c r="Q14" s="11">
         <f t="shared" si="4"/>
         <v>8068.881022793681</v>
       </c>
-      <c r="R14" s="14">
+      <c r="R14" s="11">
         <f t="shared" si="5"/>
         <v>322.75524091174725</v>
       </c>
-      <c r="S14" s="14">
+      <c r="S14" s="11">
         <f t="shared" si="6"/>
         <v>-40344.405113968409</v>
       </c>
@@ -4734,29 +4940,29 @@
       <c r="C15" s="6"/>
     </row>
     <row r="16" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="str">
+      <c r="A16" s="30" t="str">
         <f>"Attack points: 4 * sqrt(ForceMod) for each strike; "&amp;ROUND(B3,2)&amp;" strikes per second"</f>
         <v>Attack points: 4 * sqrt(ForceMod) for each strike; 3 strikes per second</v>
       </c>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7" t="s">
+      <c r="B16" s="30"/>
+      <c r="C16" s="30"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="8"/>
-      <c r="L16" s="19" t="s">
+      <c r="H16" s="30"/>
+      <c r="I16" s="30"/>
+      <c r="J16" s="30"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="M16" s="19"/>
-      <c r="N16" s="19"/>
-      <c r="O16" s="19"/>
-      <c r="P16" s="19"/>
+      <c r="M16" s="26"/>
+      <c r="N16" s="26"/>
+      <c r="O16" s="26"/>
+      <c r="P16" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -4808,7 +5014,7 @@
   <dimension ref="A1:Q16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:F2"/>
+      <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4825,10 +5031,10 @@
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="12"/>
+      <c r="F2" s="22"/>
       <c r="H2" s="4" t="s">
         <v>16</v>
       </c>
@@ -4840,51 +5046,51 @@
       <c r="B3" s="5">
         <v>3</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="E3" s="13" t="s">
         <v>16</v>
       </c>
       <c r="F3" t="s">
         <v>30</v>
       </c>
-      <c r="G3" s="17" t="s">
+      <c r="G3" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="17" t="s">
+      <c r="H3" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
-      <c r="L3" s="17" t="str">
+      <c r="I3" s="13"/>
+      <c r="J3" s="13"/>
+      <c r="L3" s="13" t="str">
         <f>E3</f>
         <v>Ebony</v>
       </c>
-      <c r="M3" s="17" t="str">
+      <c r="M3" s="13" t="str">
         <f t="shared" ref="M3:Q3" si="0">F3</f>
         <v>Red</v>
       </c>
-      <c r="N3" s="17" t="str">
+      <c r="N3" s="13" t="str">
         <f t="shared" si="0"/>
         <v>Oak</v>
       </c>
-      <c r="O3" s="17" t="str">
+      <c r="O3" s="13" t="str">
         <f t="shared" si="0"/>
         <v>Birch</v>
       </c>
-      <c r="P3" s="17">
+      <c r="P3" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q3" s="17">
+      <c r="Q3" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
       <c r="E4">
         <v>19</v>
       </c>
@@ -4908,33 +5114,34 @@
       <c r="C5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="29" t="str">
+      <c r="E5" s="23" t="str">
         <f>E2&amp;" to take one tile"</f>
         <v>Seconds take to take one tile</v>
       </c>
-      <c r="F5" s="29"/>
-      <c r="G5" s="29"/>
-      <c r="H5" s="29"/>
-      <c r="I5" s="29"/>
-      <c r="J5" s="29"/>
-      <c r="L5" s="30" t="s">
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="23"/>
+      <c r="I5" s="23"/>
+      <c r="J5" s="23"/>
+      <c r="L5" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="M5" s="30"/>
-      <c r="N5" s="30"/>
-      <c r="O5" s="30"/>
-      <c r="P5" s="30"/>
-      <c r="Q5" s="30"/>
+      <c r="M5" s="25"/>
+      <c r="N5" s="25"/>
+      <c r="O5" s="25"/>
+      <c r="P5" s="25"/>
+      <c r="Q5" s="25"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="31" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" s="31">
+      <c r="A6" s="21" t="str">
+        <f>Table3[[#This Row],[Material]]</f>
+        <v>Stone</v>
+      </c>
+      <c r="B6" s="21">
         <f>Table3[[#This Row],[ForceMod]]</f>
         <v>1</v>
       </c>
-      <c r="C6" s="31">
+      <c r="C6" s="21">
         <f>Table3[[#This Row],[Durability]]</f>
         <v>147</v>
       </c>
@@ -4962,40 +5169,41 @@
         <f>J$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B6))</f>
         <v>0</v>
       </c>
-      <c r="L6" s="14">
+      <c r="L6" s="11">
         <f>$C6/E$4</f>
         <v>7.7368421052631575</v>
       </c>
-      <c r="M6" s="14">
+      <c r="M6" s="11">
         <f t="shared" ref="M6:Q14" si="1">$C6/F$4</f>
         <v>8.6470588235294112</v>
       </c>
-      <c r="N6" s="14">
+      <c r="N6" s="11">
         <f t="shared" si="1"/>
         <v>9.1875</v>
       </c>
-      <c r="O6" s="14">
+      <c r="O6" s="11">
         <f t="shared" si="1"/>
         <v>9.8000000000000007</v>
       </c>
-      <c r="P6" s="14" t="e">
+      <c r="P6" s="11" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="Q6" s="14" t="e">
+      <c r="Q6" s="11" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="31" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="31">
+      <c r="A7" s="21" t="str">
+        <f>Table3[[#This Row],[Material]]</f>
+        <v>Copper</v>
+      </c>
+      <c r="B7" s="21">
         <f>Table3[[#This Row],[ForceMod]]</f>
         <v>2</v>
       </c>
-      <c r="C7" s="31">
+      <c r="C7" s="21">
         <f>Table3[[#This Row],[Durability]]</f>
         <v>350</v>
       </c>
@@ -5023,40 +5231,41 @@
         <f>J$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B7))</f>
         <v>0</v>
       </c>
-      <c r="L7" s="14">
+      <c r="L7" s="11">
         <f t="shared" ref="L7:L14" si="2">$C7/E$4</f>
         <v>18.421052631578949</v>
       </c>
-      <c r="M7" s="14">
+      <c r="M7" s="11">
         <f t="shared" si="1"/>
         <v>20.588235294117649</v>
       </c>
-      <c r="N7" s="14">
+      <c r="N7" s="11">
         <f t="shared" si="1"/>
         <v>21.875</v>
       </c>
-      <c r="O7" s="14">
+      <c r="O7" s="11">
         <f t="shared" si="1"/>
         <v>23.333333333333332</v>
       </c>
-      <c r="P7" s="14" t="e">
+      <c r="P7" s="11" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="Q7" s="14" t="e">
+      <c r="Q7" s="11" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="31" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="31">
+      <c r="A8" s="21" t="str">
+        <f>Table3[[#This Row],[Material]]</f>
+        <v>ElvenGlass</v>
+      </c>
+      <c r="B8" s="21">
         <f>Table3[[#This Row],[ForceMod]]</f>
         <v>4</v>
       </c>
-      <c r="C8" s="31">
+      <c r="C8" s="21">
         <f>Table3[[#This Row],[Durability]]</f>
         <v>287</v>
       </c>
@@ -5084,40 +5293,41 @@
         <f>J$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B8))</f>
         <v>0</v>
       </c>
-      <c r="L8" s="14">
+      <c r="L8" s="11">
         <f t="shared" si="2"/>
         <v>15.105263157894736</v>
       </c>
-      <c r="M8" s="14">
+      <c r="M8" s="11">
         <f t="shared" si="1"/>
         <v>16.882352941176471</v>
       </c>
-      <c r="N8" s="14">
+      <c r="N8" s="11">
         <f t="shared" si="1"/>
         <v>17.9375</v>
       </c>
-      <c r="O8" s="14">
+      <c r="O8" s="11">
         <f t="shared" si="1"/>
         <v>19.133333333333333</v>
       </c>
-      <c r="P8" s="14" t="e">
+      <c r="P8" s="11" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="Q8" s="14" t="e">
+      <c r="Q8" s="11" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="31" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="31">
+      <c r="A9" s="21" t="str">
+        <f>Table3[[#This Row],[Material]]</f>
+        <v>Iron</v>
+      </c>
+      <c r="B9" s="21">
         <f>Table3[[#This Row],[ForceMod]]</f>
         <v>5</v>
       </c>
-      <c r="C9" s="31">
+      <c r="C9" s="21">
         <f>Table3[[#This Row],[Durability]]</f>
         <v>497</v>
       </c>
@@ -5145,40 +5355,41 @@
         <f>J$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B9))</f>
         <v>0</v>
       </c>
-      <c r="L9" s="14">
+      <c r="L9" s="11">
         <f t="shared" si="2"/>
         <v>26.157894736842106</v>
       </c>
-      <c r="M9" s="14">
+      <c r="M9" s="11">
         <f t="shared" si="1"/>
         <v>29.235294117647058</v>
       </c>
-      <c r="N9" s="14">
+      <c r="N9" s="11">
         <f t="shared" si="1"/>
         <v>31.0625</v>
       </c>
-      <c r="O9" s="14">
+      <c r="O9" s="11">
         <f t="shared" si="1"/>
         <v>33.133333333333333</v>
       </c>
-      <c r="P9" s="14" t="e">
+      <c r="P9" s="11" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="Q9" s="14" t="e">
+      <c r="Q9" s="11" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="31" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="31">
+      <c r="A10" s="21" t="str">
+        <f>Table3[[#This Row],[Material]]</f>
+        <v>Silver</v>
+      </c>
+      <c r="B10" s="21">
         <f>Table3[[#This Row],[ForceMod]]</f>
         <v>9</v>
       </c>
-      <c r="C10" s="31">
+      <c r="C10" s="21">
         <f>Table3[[#This Row],[Durability]]</f>
         <v>319</v>
       </c>
@@ -5206,40 +5417,41 @@
         <f>J$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B10))</f>
         <v>0</v>
       </c>
-      <c r="L10" s="14">
+      <c r="L10" s="11">
         <f t="shared" si="2"/>
         <v>16.789473684210527</v>
       </c>
-      <c r="M10" s="14">
+      <c r="M10" s="11">
         <f t="shared" si="1"/>
         <v>18.764705882352942</v>
       </c>
-      <c r="N10" s="14">
+      <c r="N10" s="11">
         <f t="shared" si="1"/>
         <v>19.9375</v>
       </c>
-      <c r="O10" s="14">
+      <c r="O10" s="11">
         <f t="shared" si="1"/>
         <v>21.266666666666666</v>
       </c>
-      <c r="P10" s="14" t="e">
+      <c r="P10" s="11" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="Q10" s="14" t="e">
+      <c r="Q10" s="11" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="31" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="31">
+      <c r="A11" s="21" t="str">
+        <f>Table3[[#This Row],[Material]]</f>
+        <v>Steel</v>
+      </c>
+      <c r="B11" s="21">
         <f>Table3[[#This Row],[ForceMod]]</f>
         <v>14</v>
       </c>
-      <c r="C11" s="31">
+      <c r="C11" s="21">
         <f>Table3[[#This Row],[Durability]]</f>
         <v>606</v>
       </c>
@@ -5267,40 +5479,41 @@
         <f>J$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B11))</f>
         <v>0</v>
       </c>
-      <c r="L11" s="14">
+      <c r="L11" s="11">
         <f t="shared" si="2"/>
         <v>31.894736842105264</v>
       </c>
-      <c r="M11" s="14">
+      <c r="M11" s="11">
         <f t="shared" si="1"/>
         <v>35.647058823529413</v>
       </c>
-      <c r="N11" s="14">
+      <c r="N11" s="11">
         <f t="shared" si="1"/>
         <v>37.875</v>
       </c>
-      <c r="O11" s="14">
+      <c r="O11" s="11">
         <f t="shared" si="1"/>
         <v>40.4</v>
       </c>
-      <c r="P11" s="14" t="e">
+      <c r="P11" s="11" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="Q11" s="14" t="e">
+      <c r="Q11" s="11" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="31">
+      <c r="A12" s="21" t="str">
+        <f>Table3[[#This Row],[Material]]</f>
+        <v>ElvenAuri</v>
+      </c>
+      <c r="B12" s="21">
         <f>Table3[[#This Row],[ForceMod]]</f>
         <v>21</v>
       </c>
-      <c r="C12" s="31">
+      <c r="C12" s="21">
         <f>Table3[[#This Row],[Durability]]</f>
         <v>476</v>
       </c>
@@ -5328,40 +5541,41 @@
         <f>J$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B12))</f>
         <v>0</v>
       </c>
-      <c r="L12" s="14">
+      <c r="L12" s="11">
         <f t="shared" si="2"/>
         <v>25.05263157894737</v>
       </c>
-      <c r="M12" s="14">
+      <c r="M12" s="11">
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
-      <c r="N12" s="14">
+      <c r="N12" s="11">
         <f t="shared" si="1"/>
         <v>29.75</v>
       </c>
-      <c r="O12" s="14">
+      <c r="O12" s="11">
         <f t="shared" si="1"/>
         <v>31.733333333333334</v>
       </c>
-      <c r="P12" s="14" t="e">
+      <c r="P12" s="11" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="Q12" s="14" t="e">
+      <c r="Q12" s="11" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="31" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13" s="31">
+      <c r="A13" s="21" t="str">
+        <f>Table3[[#This Row],[Material]]</f>
+        <v>TiAlV</v>
+      </c>
+      <c r="B13" s="21">
         <f>Table3[[#This Row],[ForceMod]]</f>
         <v>33</v>
       </c>
-      <c r="C13" s="31">
+      <c r="C13" s="21">
         <f>Table3[[#This Row],[Durability]]</f>
         <v>756</v>
       </c>
@@ -5389,40 +5603,41 @@
         <f>J$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B13))</f>
         <v>0</v>
       </c>
-      <c r="L13" s="14">
+      <c r="L13" s="11">
         <f t="shared" si="2"/>
         <v>39.789473684210527</v>
       </c>
-      <c r="M13" s="14">
+      <c r="M13" s="11">
         <f t="shared" si="1"/>
         <v>44.470588235294116</v>
       </c>
-      <c r="N13" s="14">
+      <c r="N13" s="11">
         <f t="shared" si="1"/>
         <v>47.25</v>
       </c>
-      <c r="O13" s="14">
+      <c r="O13" s="11">
         <f t="shared" si="1"/>
         <v>50.4</v>
       </c>
-      <c r="P13" s="14" t="e">
+      <c r="P13" s="11" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="Q13" s="14" t="e">
+      <c r="Q13" s="11" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="31">
+      <c r="A14" s="21" t="str">
+        <f>Table3[[#This Row],[Material]]</f>
+        <v>SpcAdamant</v>
+      </c>
+      <c r="B14" s="21">
         <f>Table3[[#This Row],[ForceMod]]</f>
         <v>71</v>
       </c>
-      <c r="C14" s="31">
+      <c r="C14" s="21">
         <f>Table3[[#This Row],[Durability]]</f>
         <v>1197</v>
       </c>
@@ -5450,53 +5665,53 @@
         <f>J$4/(4*VLOOKUP($E$2,Variables!$A$1:$B$2,2,FALSE)*SQRT($B14))</f>
         <v>0</v>
       </c>
-      <c r="L14" s="14">
+      <c r="L14" s="11">
         <f t="shared" si="2"/>
         <v>63</v>
       </c>
-      <c r="M14" s="14">
+      <c r="M14" s="11">
         <f t="shared" si="1"/>
         <v>70.411764705882348</v>
       </c>
-      <c r="N14" s="14">
+      <c r="N14" s="11">
         <f t="shared" si="1"/>
         <v>74.8125</v>
       </c>
-      <c r="O14" s="14">
+      <c r="O14" s="11">
         <f t="shared" si="1"/>
         <v>79.8</v>
       </c>
-      <c r="P14" s="14" t="e">
+      <c r="P14" s="11" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="Q14" s="14" t="e">
+      <c r="Q14" s="11" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="str">
+      <c r="A16" s="30" t="str">
         <f>"Attacks: 4 * sqrt(ForceMod) for each strike; "&amp;ROUND(B3,2)&amp;" strikes per second"</f>
         <v>Attacks: 4 * sqrt(ForceMod) for each strike; 3 strikes per second</v>
       </c>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7" t="s">
+      <c r="B16" s="30"/>
+      <c r="C16" s="30"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="7" t="s">
+      <c r="H16" s="30"/>
+      <c r="I16" s="30"/>
+      <c r="J16" s="30"/>
+      <c r="K16" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="L16" s="7"/>
-      <c r="M16" s="7"/>
-      <c r="N16" s="7"/>
+      <c r="L16" s="30"/>
+      <c r="M16" s="30"/>
+      <c r="N16" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -5545,79 +5760,79 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.42578125" style="22" customWidth="1"/>
+    <col min="1" max="1" width="27.42578125" style="17" customWidth="1"/>
     <col min="2" max="2" width="9.140625" customWidth="1"/>
     <col min="4" max="5" width="9.140625" customWidth="1"/>
     <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="16" t="s">
         <v>22</v>
       </c>
       <c r="B1">
         <f>Sheet1!B3</f>
         <v>3</v>
       </c>
-      <c r="D1" s="11" t="str">
+      <c r="D1" s="10" t="str">
         <f>Sheet1!E2&amp;" to break a "&amp;LOWER(Sheet1!H2)&amp;" tile"</f>
-        <v>Seconds take to break a glass tile</v>
-      </c>
-      <c r="E1" s="11" t="str">
+        <v>Seconds take to break a stone tile</v>
+      </c>
+      <c r="E1" s="10" t="str">
         <f>"Tool life for "&amp;LOWER(Sheet1!H2)&amp;" tiles"</f>
-        <v>Tool life for glass tiles</v>
+        <v>Tool life for stone tiles</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="16" t="s">
         <v>23</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="D2" s="11" t="str">
+      <c r="D2" s="10" t="str">
         <f>'Sheet1 (2)'!E2&amp;" to break a "&amp;LOWER('Sheet1 (2)'!H2)&amp;" plank"</f>
         <v>Seconds take to break a ebony plank</v>
       </c>
-      <c r="E2" s="11" t="str">
+      <c r="E2" s="10" t="str">
         <f>"Tool life for "&amp;LOWER('Sheet1 (2)'!H2)&amp;" tiles"</f>
         <v>Tool life for ebony tiles</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="10">
+      <c r="B3" s="9">
         <f>Sheet1!B3</f>
         <v>3</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="E3" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15" t="s">
+      <c r="F3" s="31"/>
+      <c r="G3" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="H3" s="15"/>
+      <c r="H3" s="31"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="17" t="s">
         <v>37</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="D4" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="E4" s="16" t="s">
+      <c r="E4" s="12" t="s">
         <v>27</v>
       </c>
       <c r="F4" t="s">
         <v>28</v>
       </c>
-      <c r="G4" s="16" t="s">
+      <c r="G4" s="12" t="s">
         <v>27</v>
       </c>
       <c r="H4" t="s">
@@ -5625,197 +5840,197 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D5" s="11">
+      <c r="D5" s="10">
         <v>4</v>
       </c>
-      <c r="E5" s="14">
+      <c r="E5" s="11">
         <f>HLOOKUP(Sheet1!$H$2,Sheet1!$E$3:$J$14,$D5,FALSE)</f>
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="F5" s="14">
+        <v>4</v>
+      </c>
+      <c r="F5" s="11">
         <f>HLOOKUP(Sheet1!$H$2,Sheet1!$N$3:$S$14,$D5,FALSE)</f>
-        <v>117.6</v>
-      </c>
-      <c r="G5" s="14">
+        <v>12.25</v>
+      </c>
+      <c r="G5" s="11">
         <f>HLOOKUP('Sheet1 (2)'!$H$2,'Sheet1 (2)'!$E$3:$J$14,$D5,FALSE)</f>
         <v>1.5833333333333333</v>
       </c>
-      <c r="H5" s="14" t="e">
+      <c r="H5" s="11" t="e">
         <f>HLOOKUP('Sheet1 (2)'!$H$2,'Sheet1 (2)'!$N$3:$S$14,$D5,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D6" s="11">
+      <c r="D6" s="10">
         <v>5</v>
       </c>
-      <c r="E6" s="14">
+      <c r="E6" s="11">
         <f>HLOOKUP(Sheet1!$H$2,Sheet1!$E$3:$J$14,$D6,FALSE)</f>
-        <v>0.29462782549439476</v>
-      </c>
-      <c r="F6" s="14">
+        <v>2.8284271247461898</v>
+      </c>
+      <c r="F6" s="11">
         <f>HLOOKUP(Sheet1!$H$2,Sheet1!$N$3:$S$14,$D6,FALSE)</f>
-        <v>395.97979746446663</v>
-      </c>
-      <c r="G6" s="14">
+        <v>41.247895569215274</v>
+      </c>
+      <c r="G6" s="11">
         <f>HLOOKUP('Sheet1 (2)'!$H$2,'Sheet1 (2)'!$E$3:$J$14,$D6,FALSE)</f>
         <v>1.1195857368787001</v>
       </c>
-      <c r="H6" s="14" t="e">
+      <c r="H6" s="11" t="e">
         <f>HLOOKUP('Sheet1 (2)'!$H$2,'Sheet1 (2)'!$N$3:$S$14,$D6,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D7" s="11">
+      <c r="D7" s="10">
         <v>6</v>
       </c>
-      <c r="E7" s="14">
+      <c r="E7" s="11">
         <f>HLOOKUP(Sheet1!$H$2,Sheet1!$E$3:$J$14,$D7,FALSE)</f>
-        <v>0.20833333333333334</v>
-      </c>
-      <c r="F7" s="14">
+        <v>2</v>
+      </c>
+      <c r="F7" s="11">
         <f>HLOOKUP(Sheet1!$H$2,Sheet1!$N$3:$S$14,$D7,FALSE)</f>
-        <v>459.2</v>
-      </c>
-      <c r="G7" s="14">
+        <v>47.833333333333336</v>
+      </c>
+      <c r="G7" s="11">
         <f>HLOOKUP('Sheet1 (2)'!$H$2,'Sheet1 (2)'!$E$3:$J$14,$D7,FALSE)</f>
         <v>0.79166666666666663</v>
       </c>
-      <c r="H7" s="14" t="e">
+      <c r="H7" s="11" t="e">
         <f>HLOOKUP('Sheet1 (2)'!$H$2,'Sheet1 (2)'!$N$3:$S$14,$D7,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D8" s="11">
+      <c r="D8" s="10">
         <v>7</v>
       </c>
-      <c r="E8" s="14">
+      <c r="E8" s="11">
         <f>HLOOKUP(Sheet1!$H$2,Sheet1!$E$3:$J$14,$D8,FALSE)</f>
-        <v>0.18633899812498247</v>
-      </c>
-      <c r="F8" s="14">
+        <v>1.7888543819998317</v>
+      </c>
+      <c r="F8" s="11">
         <f>HLOOKUP(Sheet1!$H$2,Sheet1!$N$3:$S$14,$D8,FALSE)</f>
-        <v>889.06062785391634</v>
-      </c>
-      <c r="G8" s="14">
+        <v>92.610482068116283</v>
+      </c>
+      <c r="G8" s="11">
         <f>HLOOKUP('Sheet1 (2)'!$H$2,'Sheet1 (2)'!$E$3:$J$14,$D8,FALSE)</f>
         <v>0.70808819287493341</v>
       </c>
-      <c r="H8" s="14" t="e">
+      <c r="H8" s="11" t="e">
         <f>HLOOKUP('Sheet1 (2)'!$H$2,'Sheet1 (2)'!$N$3:$S$14,$D8,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D9" s="11">
+      <c r="D9" s="10">
         <v>8</v>
       </c>
-      <c r="E9" s="14">
+      <c r="E9" s="11">
         <f>HLOOKUP(Sheet1!$H$2,Sheet1!$E$3:$J$14,$D9,FALSE)</f>
-        <v>0.1388888888888889</v>
-      </c>
-      <c r="F9" s="14">
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="F9" s="11">
         <f>HLOOKUP(Sheet1!$H$2,Sheet1!$N$3:$S$14,$D9,FALSE)</f>
-        <v>765.6</v>
-      </c>
-      <c r="G9" s="14">
+        <v>79.75</v>
+      </c>
+      <c r="G9" s="11">
         <f>HLOOKUP('Sheet1 (2)'!$H$2,'Sheet1 (2)'!$E$3:$J$14,$D9,FALSE)</f>
         <v>0.52777777777777779</v>
       </c>
-      <c r="H9" s="14" t="e">
+      <c r="H9" s="11" t="e">
         <f>HLOOKUP('Sheet1 (2)'!$H$2,'Sheet1 (2)'!$N$3:$S$14,$D9,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D10" s="11">
+      <c r="D10" s="10">
         <v>9</v>
       </c>
-      <c r="E10" s="14">
+      <c r="E10" s="11">
         <f>HLOOKUP(Sheet1!$H$2,Sheet1!$E$3:$J$14,$D10,FALSE)</f>
-        <v>0.11135885079684349</v>
-      </c>
-      <c r="F10" s="14">
+        <v>1.0690449676496976</v>
+      </c>
+      <c r="F10" s="11">
         <f>HLOOKUP(Sheet1!$H$2,Sheet1!$N$3:$S$14,$D10,FALSE)</f>
-        <v>1813.955501108007</v>
-      </c>
-      <c r="G10" s="14">
+        <v>188.95369803208402</v>
+      </c>
+      <c r="G10" s="11">
         <f>HLOOKUP('Sheet1 (2)'!$H$2,'Sheet1 (2)'!$E$3:$J$14,$D10,FALSE)</f>
         <v>0.42316363302800525</v>
       </c>
-      <c r="H10" s="14" t="e">
+      <c r="H10" s="11" t="e">
         <f>HLOOKUP('Sheet1 (2)'!$H$2,'Sheet1 (2)'!$N$3:$S$14,$D10,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D11" s="11">
+      <c r="D11" s="10">
         <v>10</v>
       </c>
-      <c r="E11" s="14">
+      <c r="E11" s="11">
         <f>HLOOKUP(Sheet1!$H$2,Sheet1!$E$3:$J$14,$D11,FALSE)</f>
-        <v>9.0924120931663494E-2</v>
-      </c>
-      <c r="F11" s="14">
+        <v>0.87287156094396945</v>
+      </c>
+      <c r="F11" s="11">
         <f>HLOOKUP(Sheet1!$H$2,Sheet1!$N$3:$S$14,$D11,FALSE)</f>
-        <v>1745.0448246391836</v>
-      </c>
-      <c r="G11" s="14">
+        <v>181.77550256658165</v>
+      </c>
+      <c r="G11" s="11">
         <f>HLOOKUP('Sheet1 (2)'!$H$2,'Sheet1 (2)'!$E$3:$J$14,$D11,FALSE)</f>
         <v>0.34551165954032126</v>
       </c>
-      <c r="H11" s="14" t="e">
+      <c r="H11" s="11" t="e">
         <f>HLOOKUP('Sheet1 (2)'!$H$2,'Sheet1 (2)'!$N$3:$S$14,$D11,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D12" s="11">
+      <c r="D12" s="10">
         <v>11</v>
       </c>
-      <c r="E12" s="14">
+      <c r="E12" s="11">
         <f>HLOOKUP(Sheet1!$H$2,Sheet1!$E$3:$J$14,$D12,FALSE)</f>
-        <v>7.2532356648207438E-2</v>
-      </c>
-      <c r="F12" s="14">
+        <v>0.69631062382279141</v>
+      </c>
+      <c r="F12" s="11">
         <f>HLOOKUP(Sheet1!$H$2,Sheet1!$N$3:$S$14,$D12,FALSE)</f>
-        <v>3474.3114886261997</v>
-      </c>
-      <c r="G12" s="14">
+        <v>361.90744673189579</v>
+      </c>
+      <c r="G12" s="11">
         <f>HLOOKUP('Sheet1 (2)'!$H$2,'Sheet1 (2)'!$E$3:$J$14,$D12,FALSE)</f>
         <v>0.27562295526318825</v>
       </c>
-      <c r="H12" s="14" t="e">
+      <c r="H12" s="11" t="e">
         <f>HLOOKUP('Sheet1 (2)'!$H$2,'Sheet1 (2)'!$N$3:$S$14,$D12,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D13" s="11">
+      <c r="D13" s="10">
         <v>12</v>
       </c>
-      <c r="E13" s="14">
+      <c r="E13" s="11">
         <f>HLOOKUP(Sheet1!$H$2,Sheet1!$E$3:$J$14,$D13,FALSE)</f>
-        <v>4.944923575807722E-2</v>
-      </c>
-      <c r="F13" s="14">
+        <v>0.4747126632775413</v>
+      </c>
+      <c r="F13" s="11">
         <f>HLOOKUP(Sheet1!$H$2,Sheet1!$N$3:$S$14,$D13,FALSE)</f>
-        <v>8068.881022793681</v>
-      </c>
-      <c r="G13" s="14">
+        <v>840.50843987434189</v>
+      </c>
+      <c r="G13" s="11">
         <f>HLOOKUP('Sheet1 (2)'!$H$2,'Sheet1 (2)'!$E$3:$J$14,$D13,FALSE)</f>
         <v>0.18790709588069343</v>
       </c>
-      <c r="H13" s="14" t="e">
+      <c r="H13" s="11" t="e">
         <f>HLOOKUP('Sheet1 (2)'!$H$2,'Sheet1 (2)'!$N$3:$S$14,$D13,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
     </row>
   </sheetData>
   <dataConsolidate/>

</xml_diff>